<commit_message>
added code to read excel sheet
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F20B4A-A66E-4EB5-8DEA-C3348D3D4EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC7BB24-493A-4A24-8FD1-B4BC03F579E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3530" yWindow="3950" windowWidth="28800" windowHeight="15370" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>Akhetonics</t>
   </si>
   <si>
-    <t>XPU, raised 6.3 M USD but company seems like they're selling snake oil</t>
-  </si>
-  <si>
     <t>OpenAI</t>
   </si>
   <si>
@@ -545,9 +542,6 @@
     <t>Advanced heterogeneous integration, SiN, GaAs, GaN, InP</t>
   </si>
   <si>
-    <t>Black SemiCconductor</t>
-  </si>
-  <si>
     <t>&lt;200</t>
   </si>
   <si>
@@ -588,6 +582,12 @@
   </si>
   <si>
     <t>Glasgow and London and Palo Alto and  Boston and Berlin</t>
+  </si>
+  <si>
+    <t>Black Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XPU, raised 6.3 M USD </t>
   </si>
 </sst>
 </file>
@@ -637,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -646,9 +646,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -985,103 +982,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
-  <dimension ref="C1:H37"/>
+  <dimension ref="B1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="8" width="28.1640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="28.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
+    <col min="5" max="7" width="28.1640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="3:8" s="2" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" s="2" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C3" s="3" t="s">
+    <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4">
+      <c r="C3" s="1">
         <v>200</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>170</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C4" s="3" t="s">
+    <row r="4" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4">
+      <c r="C4" s="1">
         <v>200</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C6" s="3" t="s">
+    <row r="6" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="4">
+      <c r="C6" s="1">
         <v>280</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>46</v>
@@ -1092,36 +1094,36 @@
       <c r="G6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="1" t="s">
+    </row>
+    <row r="7" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="3" t="s">
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="4">
+      <c r="G7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="1" t="s">
+    </row>
+    <row r="8" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>55</v>
@@ -1129,67 +1131,67 @@
       <c r="F8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="1" t="s">
+    </row>
+    <row r="9" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="4">
-        <v>20</v>
-      </c>
       <c r="E9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="1" t="s">
+    </row>
+    <row r="10" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="1" t="s">
+    </row>
+    <row r="11" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>68</v>
@@ -1197,83 +1199,83 @@
       <c r="F12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="1" t="s">
+    </row>
+    <row r="13" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D13" s="4">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="3" t="s">
+    </row>
+    <row r="14" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" s="1" t="s">
+    </row>
+    <row r="17" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1282,226 +1284,226 @@
       <c r="F17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C18" s="3" t="s">
+    </row>
+    <row r="18" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>99</v>
+      <c r="D18" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C19" s="3" t="s">
+    </row>
+    <row r="19" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="E20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C21" s="3" t="s">
+    </row>
+    <row r="21" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C22" s="3" t="s">
+    </row>
+    <row r="22" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="1">
+        <v>50</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="4">
-        <v>50</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" ht="34" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C23" s="3" t="s">
+    </row>
+    <row r="23" spans="2:7" ht="34" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H23" s="1" t="s">
+    </row>
+    <row r="24" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C24" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" s="1" t="s">
+    <row r="25" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="E25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F25" s="1" t="s">
+    </row>
+    <row r="26" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F26" s="1" t="s">
+    </row>
+    <row r="27" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G27" s="1" t="s">
+    </row>
+    <row r="28" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="28" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C28" s="3" t="s">
+      <c r="E28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C29" s="3" t="s">
+    </row>
+    <row r="29" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C30" s="3" t="s">
+    </row>
+    <row r="30" spans="2:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>161</v>
@@ -1509,36 +1511,33 @@
       <c r="F30" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G30" s="1" t="s">
+    </row>
+    <row r="31" spans="2:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="3:8" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C31" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="E31" s="1" t="s">
+    <row r="32" spans="2:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="F32" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="33" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1609,96 +1608,96 @@
     </row>
     <row r="7" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C14" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C15" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C16" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D16" s="1">
         <v>500</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" s="4" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="1">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D17" s="4">
-        <v>100</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>182</v>
+      <c r="G17" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="3:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C18" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="3:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C19" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="3:7" ht="28" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C20" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="21" spans="3:7" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1783,23 +1782,23 @@
     </row>
     <row r="10" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1861,13 +1860,13 @@
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>22</v>
@@ -1878,32 +1877,32 @@
         <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Updated readme, added code to allow for companies to have multiple locations.
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC7BB24-493A-4A24-8FD1-B4BC03F579E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55459D3-5839-438C-A154-C0253C0072A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3530" yWindow="3950" windowWidth="28800" windowHeight="15370" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="177">
   <si>
     <t>Company Name</t>
   </si>
@@ -59,12 +59,6 @@
     <t>Optical MVM / PNN</t>
   </si>
   <si>
-    <t xml:space="preserve">Location </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HT works here. </t>
-  </si>
-  <si>
     <t>Lightelligence</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t xml:space="preserve">Optical I/O for AI, Interconnection </t>
   </si>
   <si>
-    <t>Nvidia, Intel, AMD investors</t>
-  </si>
-  <si>
     <t>Mark Wade</t>
   </si>
   <si>
@@ -185,15 +176,9 @@
     <t>Palo Alto, CA</t>
   </si>
   <si>
-    <t>HT used to work here</t>
-  </si>
-  <si>
     <t>solid-state quantum processor</t>
   </si>
   <si>
-    <t>Thomas works here</t>
-  </si>
-  <si>
     <t>Shmuel Bachinsky</t>
   </si>
   <si>
@@ -326,9 +311,6 @@
     <t>Murray Hill, New Jersey, USA</t>
   </si>
   <si>
-    <t>Sara and Siamik work/worked here</t>
-  </si>
-  <si>
     <t>Peter Winzer, Bell Labs</t>
   </si>
   <si>
@@ -476,9 +458,6 @@
     <t>photonic quantum processor based upon silicon nitride waveguides</t>
   </si>
   <si>
-    <t>Ulm/Stuttgart Germany, Amsterdam/Enschede Netherlands</t>
-  </si>
-  <si>
     <t>photonic quantum technology components</t>
   </si>
   <si>
@@ -527,12 +506,6 @@
     <t>Matt Streshinsky, Came out of Lumious Computing</t>
   </si>
   <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Goleta, Californi</t>
-  </si>
-  <si>
     <t>Nexus Photonics</t>
   </si>
   <si>
@@ -551,9 +524,6 @@
     <t>Aachen, Germany</t>
   </si>
   <si>
-    <t>Mountain View, CA and Toronto, CAN, and Boston, MA</t>
-  </si>
-  <si>
     <t>Boston, MA</t>
   </si>
   <si>
@@ -587,7 +557,19 @@
     <t>Black Semiconductor</t>
   </si>
   <si>
-    <t xml:space="preserve">XPU, raised 6.3 M USD </t>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Mountain View, CA and Toronto, Canada, and Boston, MA</t>
+  </si>
+  <si>
+    <t>Ulm, Germany and Stuttgart Germany, and Amsterdam, Netherlands, and Enschede, Netherlands</t>
+  </si>
+  <si>
+    <t>California,USA</t>
+  </si>
+  <si>
+    <t>Goleta, California, USA</t>
   </si>
 </sst>
 </file>
@@ -982,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
-  <dimension ref="B1:G37"/>
+  <dimension ref="B1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -993,12 +975,12 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="3" width="28.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="7" width="28.1640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="28.1640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:7" s="2" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1009,16 +991,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1029,515 +1008,494 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>200</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1">
         <v>280</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C7" s="1">
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
         <v>100</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="1" t="s">
+    </row>
+    <row r="11" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="3" t="s">
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="3" t="s">
+      <c r="E12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="13" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="C13" s="1">
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="F17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="3" t="s">
+    </row>
+    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="3" t="s">
+      <c r="C20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="E20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="1" t="s">
+    </row>
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="C22" s="1">
         <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="34" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="34" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="3" t="s">
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="3" t="s">
+      <c r="C25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="1" t="s">
+    </row>
+    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="1" t="s">
+    </row>
+    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="3" t="s">
+      <c r="F27" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="E28" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="1" t="s">
+    </row>
+    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="3" t="s">
+      <c r="D29" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C29" s="1" t="s">
+    </row>
+    <row r="30" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="3" t="s">
+      <c r="D31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="33" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1552,158 +1510,158 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
-  <dimension ref="C1:H24"/>
+  <dimension ref="B1:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="8" width="28.1640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.1640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>172</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="1" t="s">
+    <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="1" t="s">
+    <row r="9" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C13" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C15" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C16" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="1">
+    <row r="11" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="1">
         <v>500</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="1">
+        <v>100</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="1">
-        <v>100</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C18" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" ht="28" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="3:7" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="3:7" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="3:7" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1711,109 +1669,109 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3E1C2-3C44-2549-B6BE-21FD6EE1DD33}">
-  <dimension ref="C1:H25"/>
+  <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="8" width="28.1640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.1640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>172</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="1" t="s">
+    <row r="7" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="1" t="s">
+    <row r="8" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="1" t="s">
+    <row r="9" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C10" s="1" t="s">
-        <v>75</v>
+    <row r="10" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C12" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" s="1" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" s="1" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" s="1" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="17" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1821,109 +1779,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
-  <dimension ref="C1:H25"/>
+  <dimension ref="B1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="8" width="28.1640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.1640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:8" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>172</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>163</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>167</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="C5" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="3:8" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" s="1" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" s="1" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" s="1" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="17" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
use geopy to take array of rough location and get actual Long/Lat coordinates for vizualization
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55459D3-5839-438C-A154-C0253C0072A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387A30F0-103D-4995-8236-6002C248D055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="19020" yWindow="0" windowWidth="19380" windowHeight="20880" activeTab="3" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -966,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1512,7 +1512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
   <dimension ref="B1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1781,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
   <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Used Folium to map companies (current small/startup only)
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\Career_Materials\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387A30F0-103D-4995-8236-6002C248D055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2899779C-4F9B-44BF-91CA-2080A77BBF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19020" yWindow="0" windowWidth="19380" windowHeight="20880" activeTab="3" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="0" yWindow="615" windowWidth="24150" windowHeight="14985" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="178">
   <si>
     <t>Company Name</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Lukas Chrostowski</t>
   </si>
   <si>
-    <t>Vancover, BC, Canada</t>
-  </si>
-  <si>
     <t>Packaging and Layout Design; world’s best chipsets for integrated photonics</t>
   </si>
   <si>
@@ -413,9 +410,6 @@
     <t>CLOSED 11/2024</t>
   </si>
   <si>
-    <t>London, Toronto, Austin</t>
-  </si>
-  <si>
     <t>Orca Computing</t>
   </si>
   <si>
@@ -434,9 +428,6 @@
     <t>Silicon photonic Quantum Computing</t>
   </si>
   <si>
-    <t>Vancouver, Canada</t>
-  </si>
-  <si>
     <t>Paul Terry, Stephanie Simmons, Simon Fraser University</t>
   </si>
   <si>
@@ -570,6 +561,19 @@
   </si>
   <si>
     <t>Goleta, California, USA</t>
+  </si>
+  <si>
+    <t>London, UK and Toronto, Canada, and Austin, Tx, USA</t>
+  </si>
+  <si>
+    <t>Vancouver, BC, Canada</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Michael Kissner, 
+Leonardo Del Bino</t>
   </si>
 </sst>
 </file>
@@ -966,21 +970,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="28.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="3" width="28.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.1640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="28.125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -994,10 +998,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1011,10 +1015,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1028,10 +1032,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
@@ -1065,7 +1069,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>47</v>
       </c>
@@ -1082,7 +1086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1099,7 +1103,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1116,12 +1120,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>56</v>
@@ -1133,12 +1137,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>59</v>
@@ -1150,12 +1154,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>62</v>
@@ -1167,7 +1171,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>65</v>
       </c>
@@ -1175,334 +1179,341 @@
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="1" t="s">
+    </row>
+    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" s="1">
         <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="34" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="2:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="1" t="s">
+    </row>
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="3" t="s">
+      <c r="E25" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="F25" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="3" t="s">
+    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="3" t="s">
+      <c r="F27" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="E28" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E28" s="1" t="s">
+    </row>
+    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B29" s="3" t="s">
+      <c r="D29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E29" s="1" t="s">
+    </row>
+    <row r="30" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="3" t="s">
+      <c r="F31" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F31" s="1" t="s">
+    </row>
+    <row r="33" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1516,15 +1527,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.1640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1538,130 +1549,130 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C16" s="1">
         <v>500</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="1">
         <v>100</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    </row>
+    <row r="21" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1675,15 +1686,15 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.1640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1697,81 +1708,81 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1781,19 +1792,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
   <dimension ref="B1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.1640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1807,81 +1818,81 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" ht="56" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added information on foundries within the database, made the get coordinates function more robust to various inputs and long lists, updated icon colors.
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\Career_Materials\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2899779C-4F9B-44BF-91CA-2080A77BBF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7206F6CD-7BF2-4B2C-9809-B3CBB15AD347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="615" windowWidth="24150" windowHeight="14985" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="0" yWindow="615" windowWidth="24150" windowHeight="14985" activeTab="1" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="241">
   <si>
     <t>Company Name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Focus</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>LightMatter</t>
   </si>
   <si>
@@ -98,15 +95,9 @@
     <t>Photonic Systems Inc</t>
   </si>
   <si>
-    <t>Baton Rouge, LA</t>
-  </si>
-  <si>
     <t>Microwave Photonics, Neuromorphioc Photonics</t>
   </si>
   <si>
-    <t>Nvidia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Google </t>
   </si>
   <si>
@@ -122,24 +113,12 @@
     <t>Global Foundries</t>
   </si>
   <si>
-    <t xml:space="preserve">AIM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMF </t>
-  </si>
-  <si>
     <t xml:space="preserve">HHI </t>
   </si>
   <si>
     <t>Smart Photonics</t>
   </si>
   <si>
-    <t>LionX</t>
-  </si>
-  <si>
-    <t>Tower</t>
-  </si>
-  <si>
     <t>NEC</t>
   </si>
   <si>
@@ -260,9 +239,6 @@
     <t>&lt; 50</t>
   </si>
   <si>
-    <t>NY, USA</t>
-  </si>
-  <si>
     <t>Optelligence</t>
   </si>
   <si>
@@ -347,9 +323,6 @@
     <t>NeoPhotonics</t>
   </si>
   <si>
-    <t>Honeywell</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coherent Inc. </t>
   </si>
   <si>
@@ -507,9 +480,6 @@
   </si>
   <si>
     <t>&lt;200</t>
-  </si>
-  <si>
-    <t>2D material graphene to create ultra-fast, energy-efficient, and scalable chip fabrics</t>
   </si>
   <si>
     <t>Aachen, Germany</t>
@@ -574,6 +544,225 @@
   <si>
     <t>Michael Kissner, 
 Leonardo Del Bino</t>
+  </si>
+  <si>
+    <t>Tin Komljenovic, Chong Zhang, John Bowers, UCSB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Daniel Schall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D material graphene to create ultra-fast, energy-efficient, and scalable chip fabrics, Graphene-based photonic modulator / detector </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circuit Research Group </t>
+  </si>
+  <si>
+    <t>Tom Gray: Head of CRG</t>
+  </si>
+  <si>
+    <t>Nvidia Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Clara, California and Seattle, Washington </t>
+  </si>
+  <si>
+    <t>Mountain View, California and Zürich, Switzerland and Seattle, Washington and San Francisco, CA</t>
+  </si>
+  <si>
+    <t>Google Quantum AI + Taara @ Google X + Google Platforms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantum: Hartmut Neven, Taara: Mahesh Krishnaswamy </t>
+  </si>
+  <si>
+    <t>300+</t>
+  </si>
+  <si>
+    <t>70+</t>
+  </si>
+  <si>
+    <t>Fiber Sensing, Optical Compute, Fiber Telecommunication Optimization</t>
+  </si>
+  <si>
+    <t>Princeton, NJ</t>
+  </si>
+  <si>
+    <t>Optical input/output (I/O) technology innovation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Clara, California and Hillsboro, Oregon </t>
+  </si>
+  <si>
+    <t>Richard Uhlig</t>
+  </si>
+  <si>
+    <t>Ewing Township, NJ</t>
+  </si>
+  <si>
+    <t>President: Chris White, ONS Head: Ting Wang, Princeton University</t>
+  </si>
+  <si>
+    <t>Sherwin Seligsohn, Stephen Forrest, Princeton University</t>
+  </si>
+  <si>
+    <t>OLED technology, Tangential interest in optical compute</t>
+  </si>
+  <si>
+    <t>Billerica, MA</t>
+  </si>
+  <si>
+    <t>Newark, DE, USA</t>
+  </si>
+  <si>
+    <t>New York, NY, USA</t>
+  </si>
+  <si>
+    <t>Baton Rouge, LA and St. Louis, MO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FDX™ FD-SOI, Silicon Photonics, RF SOI, BCD &amp; BCDLite, Bulk CMOS, FinFET 12LP+, SiGe</t>
+  </si>
+  <si>
+    <t>CEO: Thomas Caulfield and Si Ph lead: Kevin Soukup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Albany, NY and Rochester, NY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIM Photonics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active/Passive Si, Electronic Interposer, Low-Loss Active Si, Quantum Flex, SiN, Active Interposer, III-V, SiN Visible  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singapore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced Micro Foundry (AMF) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOI, 800nm SiN on SOI, CoPackaging,  </t>
+  </si>
+  <si>
+    <t>CEO Wade Cook, Ph  Dir: Chris Baiocco, SUNY</t>
+  </si>
+  <si>
+    <t>CEO Jagadish CV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Head of Ph  Klemens Janiak. </t>
+  </si>
+  <si>
+    <t>MPW, InP, RF PIC</t>
+  </si>
+  <si>
+    <t>Berlin, Germany and Goslar, Germany</t>
+  </si>
+  <si>
+    <t>300 </t>
+  </si>
+  <si>
+    <t>Eindhoven,  Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPW, InP </t>
+  </si>
+  <si>
+    <t>CEO Johan Feenstra, VP R&amp;D Yuval Kariv</t>
+  </si>
+  <si>
+    <t>190 </t>
+  </si>
+  <si>
+    <t>SiN TriPleX , Visible, 1550nm, MEMs</t>
+  </si>
+  <si>
+    <t>CEO Arne Leinse, CTO Ronald Dekker,</t>
+  </si>
+  <si>
+    <t>LioniX</t>
+  </si>
+  <si>
+    <t>Enschede, Netherlands</t>
+  </si>
+  <si>
+    <t>Tower Semiconductor</t>
+  </si>
+  <si>
+    <t>200mm Si, SiN, Darpa LUMOS,  RF, CMOS, MEMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEO Russell C. Ellwanger, </t>
+  </si>
+  <si>
+    <t>CMC Microsystems</t>
+  </si>
+  <si>
+    <t>CEO: Gordon Harling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All-Nitride-Core Photonics, </t>
+  </si>
+  <si>
+    <t>X-Fab</t>
+  </si>
+  <si>
+    <t>TFLN, Hybrid Integration, Heterogenenous Intergration, High depth Si, Packaging</t>
+  </si>
+  <si>
+    <t>CEO Antti Vasara</t>
+  </si>
+  <si>
+    <t>Otaniemi Espoo Finland</t>
+  </si>
+  <si>
+    <t>2,355 </t>
+  </si>
+  <si>
+    <t>200nm CMOS+Si, 300nm CMOS+Si, MPW, Volume, SiN, Packaging, Research</t>
+  </si>
+  <si>
+    <t>CEO Luc Van den hove and CTO Ilan Spillinger</t>
+  </si>
+  <si>
+    <t>Canadian consortium for integrated photonics and packaging</t>
+  </si>
+  <si>
+    <t>JePPiX</t>
+  </si>
+  <si>
+    <t>103 </t>
+  </si>
+  <si>
+    <t>Montreal, Canada and Kingston, Canada and Ottawa, Canada</t>
+  </si>
+  <si>
+    <t>Lubbock, USA and Corbeil-Essonnes, France and Itzehoe, Germany and Dresden Germany, and Erfurt Germany, and Kuching, Malaysia</t>
+  </si>
+  <si>
+    <t>350nm - 130nm CMOS, RF MEMS,  SIC, GaN, Microfluidics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEO: Rudi De Winter, </t>
+  </si>
+  <si>
+    <t>European consortium for integrated photonics</t>
+  </si>
+  <si>
+    <t>CEO: Francisco Rodrigues</t>
+  </si>
+  <si>
+    <t>Eindhoven, Netherlands</t>
+  </si>
+  <si>
+    <t>Migdal Haemek, Israel and Newport Beach, CA, USA and  San Antonio, Texas and Hokuriku, Japan and Agrate, Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leuven, Belgium and San Francisco, CA and Kissimmee, FL and Berkeley, CA and San Jose, CA and Eindhoven, Netherlands, and Antwerp, Netherlands and Chicago, IL, USA, and Ann Harbor, Michigan, and West Lafayette, IN </t>
+  </si>
+  <si>
+    <t>Austin, Texas and Dallas, Texas and Essex Junction, Vermont and Malta, New York and New York, New York and Santa Clara, California and San Diego, California and Dresden, Germany and Leuven Belgium and Munich, Germany and Sofia, Bulgaria and Bengaluru, India and Hsinchu, Taiwan and Malaysia and Shanghai, China and Seoul, South Korea and Singapore and Yokohama, Japan</t>
   </si>
 </sst>
 </file>
@@ -623,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -632,6 +821,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -970,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -995,521 +1190,527 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1">
         <v>200</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>200</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1">
         <v>280</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1">
         <v>100</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1">
         <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1">
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>73</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C22" s="1">
         <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>156</v>
+        <v>170</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1521,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
-  <dimension ref="B1:G24"/>
+  <dimension ref="B1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1534,8 +1735,8 @@
     <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1546,127 +1747,184 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1">
+        <v>700</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1">
+        <v>470</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C16" s="1">
         <v>500</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C17" s="1">
         <v>100</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1680,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3E1C2-3C44-2549-B6BE-21FD6EE1DD33}">
-  <dimension ref="B1:G25"/>
+  <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1693,8 +1951,8 @@
     <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1705,75 +1963,234 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5">
+        <v>13000</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="C4" s="1">
+        <v>500</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="C5" s="1">
+        <v>130</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="C8" s="1">
+        <v>70</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="C9" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>131</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5500</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="5">
+        <v>4500</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15" s="1">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1790,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
-  <dimension ref="B1:G25"/>
+  <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1803,8 +2220,8 @@
     <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1815,75 +2232,74 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:7" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>152</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added dynamically scaling legend (responds to flags), completed database entries for companies currently listed
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\Career_Materials\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F657E0-5931-4DA5-9BEA-6716CDB10670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4C86A4-EE08-495D-8970-9451CF52B957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="615" windowWidth="24150" windowHeight="14985" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="3" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="292">
   <si>
     <t>Company Name</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Smart Photonics</t>
   </si>
   <si>
-    <t>NEC</t>
-  </si>
-  <si>
     <t xml:space="preserve">Intel </t>
   </si>
   <si>
@@ -299,9 +296,6 @@
     <t>LiDAR</t>
   </si>
   <si>
-    <t>New York, NY 10018</t>
-  </si>
-  <si>
     <t>Steven Miller, Michel Lipson</t>
   </si>
   <si>
@@ -320,15 +314,6 @@
     <t>Scott Dufferwiel, Univ. of Sheffield</t>
   </si>
   <si>
-    <t>NeoPhotonics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coherent Inc. </t>
-  </si>
-  <si>
-    <t>Hamamatsu Corporation</t>
-  </si>
-  <si>
     <t>Nu-quantum</t>
   </si>
   <si>
@@ -347,9 +332,6 @@
     <t xml:space="preserve">Michael Geiselmann, Michael Zervas,  Tobias Kippenberg,  EPFL </t>
   </si>
   <si>
-    <t>NJ, USA and Japan</t>
-  </si>
-  <si>
     <t>Miraex</t>
   </si>
   <si>
@@ -365,12 +347,6 @@
     <t>M Squared </t>
   </si>
   <si>
-    <t>quantum technology, biophotonics, and chemical sensing</t>
-  </si>
-  <si>
-    <t>GRAEME MALCOLM OBE, Strathclyde University</t>
-  </si>
-  <si>
     <t>NTT</t>
   </si>
   <si>
@@ -458,9 +434,6 @@
     <t>Synopsys Photonic Solutions</t>
   </si>
   <si>
-    <t>Mountain View, California</t>
-  </si>
-  <si>
     <t>Enosemi</t>
   </si>
   <si>
@@ -534,9 +507,6 @@
   </si>
   <si>
     <t>Vancouver, BC, Canada</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Michael Kissner, 
@@ -576,15 +546,9 @@
     <t>300+</t>
   </si>
   <si>
-    <t>70+</t>
-  </si>
-  <si>
     <t>Fiber Sensing, Optical Compute, Fiber Telecommunication Optimization</t>
   </si>
   <si>
-    <t>Princeton, NJ</t>
-  </si>
-  <si>
     <t>Optical input/output (I/O) technology innovation</t>
   </si>
   <si>
@@ -735,9 +699,6 @@
     <t>Montreal, Canada and Kingston, Canada and Ottawa, Canada</t>
   </si>
   <si>
-    <t>Lubbock, USA and Corbeil-Essonnes, France and Itzehoe, Germany and Dresden Germany, and Erfurt Germany, and Kuching, Malaysia</t>
-  </si>
-  <si>
     <t>350nm - 130nm CMOS, RF MEMS,  SIC, GaN, Microfluidics</t>
   </si>
   <si>
@@ -756,13 +717,206 @@
     <t>Migdal Haemek, Israel and Newport Beach, CA, USA and  San Antonio, Texas and Hokuriku, Japan and Agrate, Italy</t>
   </si>
   <si>
-    <t xml:space="preserve">Leuven, Belgium and San Francisco, CA and Kissimmee, FL and Berkeley, CA and San Jose, CA and Eindhoven, Netherlands, and Antwerp, Netherlands and Chicago, IL, USA, and Ann Harbor, Michigan, and West Lafayette, IN </t>
-  </si>
-  <si>
     <t>Austin, Texas and Dallas, Texas and Essex Junction, Vermont and Malta, New York and New York, New York and Santa Clara, California and San Diego, California and Dresden, Germany and Leuven Belgium and Munich, Germany and Sofia, Bulgaria and Bengaluru, India and Hsinchu, Taiwan and Malaysia and Shanghai, China and Seoul, South Korea and Singapore and Yokohama, Japan</t>
   </si>
   <si>
     <t>San Francisco, CA and Toronto, Canada</t>
+  </si>
+  <si>
+    <t>OpenAI is an AI research and deployment company. Potentially interested in optical interconnect and MVM</t>
+  </si>
+  <si>
+    <t>CEO: Sam Altman</t>
+  </si>
+  <si>
+    <t>San Francisco, California</t>
+  </si>
+  <si>
+    <t>Cupertino, California and Austin, Texas and Boulder, Colorado and Cork, Ireland</t>
+  </si>
+  <si>
+    <t>CEO: Tim Cook and VP of Hardware John Ternus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biophotonics, Interconnections, Periscope Lens, Senors, </t>
+  </si>
+  <si>
+    <t>Rockley Photonic</t>
+  </si>
+  <si>
+    <t>Pasadena, CA</t>
+  </si>
+  <si>
+    <t>photonics chipset developer/supplier for high-volume sensor and communication products.</t>
+  </si>
+  <si>
+    <t>CEO: Richard Meier</t>
+  </si>
+  <si>
+    <t>hown an interest in photonic technologies and the benefits of ultra-fast data communication</t>
+  </si>
+  <si>
+    <t>Production-Grade Photonic Foundry for Thin-Film Lithium Niobate</t>
+  </si>
+  <si>
+    <t>Schlieren, Switzerland</t>
+  </si>
+  <si>
+    <t>Lightiium</t>
+  </si>
+  <si>
+    <t>CEO Amir Ghadimi</t>
+  </si>
+  <si>
+    <t>Hewlett Packard Labs</t>
+  </si>
+  <si>
+    <t>HP and Ayar Labs to co-develop silicon photonics-based optical I/O for HPC and AI</t>
+  </si>
+  <si>
+    <t>Leo Space Photonics</t>
+  </si>
+  <si>
+    <t>Optical Transceivers for Satellite Communications</t>
+  </si>
+  <si>
+    <t>Agia Paraskevi, Athens, Greece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leontios Stampoulidis, Ahmed Osman </t>
+  </si>
+  <si>
+    <t>III-V Lab</t>
+  </si>
+  <si>
+    <t>Everything III-V, epitazy, wafer processing, packaging, test and measurement and design support</t>
+  </si>
+  <si>
+    <t>CEO Jean-Pierre Hamaide</t>
+  </si>
+  <si>
+    <t>Palaiseau, France</t>
+  </si>
+  <si>
+    <t>Palo Alto, California and Grenoble, France</t>
+  </si>
+  <si>
+    <t>CTO Tolga Kurtoglu</t>
+  </si>
+  <si>
+    <t>Design Software and Assistance for photonic integrated circuits, OptoDesigner</t>
+  </si>
+  <si>
+    <t>Mountain View, California and Montreal, Quebec, Canada</t>
+  </si>
+  <si>
+    <t>CEO Sassine Ghazi</t>
+  </si>
+  <si>
+    <t>NEC Laboratories</t>
+  </si>
+  <si>
+    <t>Princeton, NJ and Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Yorktown Heights, New York, USA and Albany, New York, USA and Sydney, Australia  and Zurich, Switzerland</t>
+  </si>
+  <si>
+    <t>Quantum Photonics, Integrated Photonics for intereconnects, potential interest in photonics for AI, Co-packaged optics</t>
+  </si>
+  <si>
+    <t>CEO ​​​​​Arvind Krishna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Yoshihisa Yamamoto, Director, PHI Lab</t>
+  </si>
+  <si>
+    <t>Telecommunication, Research within Photonic Neural Networks and Photonic Accelerators</t>
+  </si>
+  <si>
+    <t>Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>CEO: Lisa T. Su</t>
+  </si>
+  <si>
+    <t>Quantum technology, biophotonics, and chemical sensing</t>
+  </si>
+  <si>
+    <t>Graeme Malcolm Obe, Strathclyde University</t>
+  </si>
+  <si>
+    <t>Semiconductor Manufacturing, Spectroscopy, Quantum Sensors,</t>
+  </si>
+  <si>
+    <t>Bridgewater, New Jersey and Hamamatsu, Japan and Shanghai, China and Bad Homburg, Germany</t>
+  </si>
+  <si>
+    <t>Hamamatsu Photonics</t>
+  </si>
+  <si>
+    <t>CEO: Katsuhiro Kobayashi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photonic Quantum, Integrated Photonics for Networking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silicon Valley, California, USA and Bangalore, India and Beijing, China and Ottawa, Canada and Paris, France and Vimercate, Italy </t>
+  </si>
+  <si>
+    <t>CEO: Chuck Robbins</t>
+  </si>
+  <si>
+    <t>Founders: Axel Scherer, Michael Hochberg, Tom Baehr-Jones, Eli Yablonovitch | Caltech | Acquired by Cisco</t>
+  </si>
+  <si>
+    <t>San Diego, California, USA</t>
+  </si>
+  <si>
+    <t>Si Ph Optical Transceivers, 800G tranceivers</t>
+  </si>
+  <si>
+    <t>III-V Optical Transceivers, PIC Design, Advanced Packaging, Analog Electronics, ASIC Design</t>
+  </si>
+  <si>
+    <t>San Jose, California and Ottawa, ON, Canada and Stockhom Sweden and Munich, Germany and Lisbon, Portugal and Madrid, Spain and Warsaw, Poland and Zhubei, Taiwan</t>
+  </si>
+  <si>
+    <t>CEO David W. Heard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lumentum </t>
+  </si>
+  <si>
+    <t>optical components, lasers, modulators. Aquired NeoPhotonics</t>
+  </si>
+  <si>
+    <t>San Jose, California, USA and Ottawa ON, Canada and Kanagawa, Japan and Shenzhen, Guangdong, China and Towcester, England</t>
+  </si>
+  <si>
+    <t>CEO: Alan S. Low</t>
+  </si>
+  <si>
+    <t>CEO: Mark E. Fisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coherent Corp. </t>
+  </si>
+  <si>
+    <t>Optical transceivers and many optical devices</t>
+  </si>
+  <si>
+    <t>Sunnyvale, CA, USA and Santa Clara, CA and Dallas, TX, USA and Bloomfield, CT, and Tuscon, Arizona and Hillsboro, Oregon and Düsseldorf, Germany</t>
+  </si>
+  <si>
+    <t>Santa Clara, California and Austin, Texas and Markham, Ontario, Canada and Boxborough, MA and Bangalore, India and Shanghai, China and Beijing, China</t>
+  </si>
+  <si>
+    <t>Lubbock, USA and Corbeil-Essonnes, France and Itzehoe, Germany and Dresden, Germany and Erfurt, Germany and Kuching, Malaysia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leuven, Belgium and San Francisco, CA and Kissimmee, FL and Berkeley, CA and San Jose, CA and Eindhoven, Netherlands and Antwerp, Netherlands and Chicago, IL, USA and Ann Harbor, Michigan and West Lafayette, IN </t>
   </si>
 </sst>
 </file>
@@ -1163,23 +1317,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
-  <dimension ref="B1:F37"/>
+  <dimension ref="B1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="3" width="28.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="28.08203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="1"/>
+    <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1193,10 +1347,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1210,10 +1364,10 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1227,10 +1381,10 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1247,7 +1401,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1255,33 +1409,33 @@
         <v>280</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1">
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1289,16 +1443,16 @@
         <v>100</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1306,415 +1460,426 @@
         <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="1" t="s">
+    </row>
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="1" t="s">
+    </row>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="3" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C13" s="1">
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
+      <c r="E20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="1" t="s">
+    </row>
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="C22" s="1">
         <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="34" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="1" t="s">
+    </row>
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
+      <c r="C24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
+      <c r="C26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="1" t="s">
+    </row>
+    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
+      <c r="E28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
+    </row>
+    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="E29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="3" t="s">
+    </row>
+    <row r="30" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="F30" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
+      <c r="D32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E35" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="5:5" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C33" s="1">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1722,21 +1887,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
-  <dimension ref="B1:F24"/>
+  <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1750,187 +1915,352 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="1">
+        <v>500</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C6" s="1">
         <v>700</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1">
         <v>470</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1500</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5">
+        <v>30000</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="5">
+        <v>8000</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1">
+        <v>150</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="5">
+        <v>700</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="C14" s="1">
+        <v>800</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1400</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>270</v>
       </c>
       <c r="C16" s="1">
         <v>500</v>
       </c>
+      <c r="D16" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="F16" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C17" s="1">
         <v>100</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>108</v>
+        <v>266</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>109</v>
+        <v>267</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="C18" s="1">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="C19" s="5">
+        <v>15000</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="C20" s="1">
+        <v>14000</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C21" s="1">
+        <v>300</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" s="1">
+        <v>500</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1941,18 +2271,18 @@
   <dimension ref="B1:F25"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1966,10 +2296,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1977,229 +2307,261 @@
         <v>13000</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="C4" s="1">
         <v>500</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C5" s="1">
         <v>130</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C8" s="1">
         <v>70</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="C9" s="5">
         <v>10000</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1">
         <v>100</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C12" s="5">
         <v>5500</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C14" s="5">
         <v>4500</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C15" s="1">
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" s="1">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C17" s="1">
+        <v>150</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2209,19 +2571,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2235,80 +2597,80 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleaned up code and added two more startups
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\Career_Materials\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4C86A4-EE08-495D-8970-9451CF52B957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9F5E6E-295E-4114-A90B-D93146C6B83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="3" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="0" yWindow="615" windowWidth="24150" windowHeight="14985" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="300">
   <si>
     <t>Company Name</t>
   </si>
@@ -917,6 +917,30 @@
   </si>
   <si>
     <t xml:space="preserve">Leuven, Belgium and San Francisco, CA and Kissimmee, FL and Berkeley, CA and San Jose, CA and Eindhoven, Netherlands and Antwerp, Netherlands and Chicago, IL, USA and Ann Harbor, Michigan and West Lafayette, IN </t>
+  </si>
+  <si>
+    <t>Xanadu.ai</t>
+  </si>
+  <si>
+    <t>Quantum Computing / Optical Comptuing, caling to one million qubits through optical networking</t>
+  </si>
+  <si>
+    <t>Toronto, Canada</t>
+  </si>
+  <si>
+    <t>ANELLO Photonics</t>
+  </si>
+  <si>
+    <t>Silicon Photonics for Fiber Optical Gyroscope tech (FOGs)</t>
+  </si>
+  <si>
+    <t>CEO: Mario Paniccia and CTO Mike Horton</t>
+  </si>
+  <si>
+    <t>Santa Clara, CA</t>
+  </si>
+  <si>
+    <t>Christian Weedbrook</t>
   </si>
 </sst>
 </file>
@@ -1319,21 +1343,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="28.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="3" width="28.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="28.125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1374,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1367,7 +1391,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1384,7 +1408,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1401,7 +1425,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1418,7 +1442,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -1435,7 +1459,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1452,7 +1476,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1469,7 +1493,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
@@ -1486,7 +1510,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1503,7 +1527,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1520,7 +1544,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1537,7 +1561,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1554,7 +1578,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1571,7 +1595,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1588,7 +1612,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
@@ -1605,7 +1629,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
@@ -1622,7 +1646,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
@@ -1639,7 +1663,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
@@ -1656,7 +1680,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
@@ -1673,7 +1697,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>97</v>
       </c>
@@ -1690,7 +1714,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="34" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
@@ -1707,7 +1731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
@@ -1724,7 +1748,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
@@ -1741,7 +1765,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
@@ -1758,7 +1782,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
@@ -1775,7 +1799,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>120</v>
       </c>
@@ -1792,7 +1816,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
@@ -1809,7 +1833,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
@@ -1826,7 +1850,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
@@ -1843,7 +1867,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>149</v>
       </c>
@@ -1860,7 +1884,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>244</v>
       </c>
@@ -1877,9 +1901,41 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C34" s="1">
+        <v>190</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C35" s="1">
+        <v>30</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1893,15 +1949,15 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1918,7 +1974,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
@@ -1935,7 +1991,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1952,7 +2008,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>257</v>
       </c>
@@ -1969,7 +2025,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1986,7 +2042,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2003,7 +2059,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2020,7 +2076,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2037,7 +2093,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2054,7 +2110,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2071,7 +2127,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2088,7 +2144,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -2105,7 +2161,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>281</v>
       </c>
@@ -2122,7 +2178,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>286</v>
       </c>
@@ -2139,7 +2195,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>270</v>
       </c>
@@ -2156,7 +2212,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2173,7 +2229,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>102</v>
       </c>
@@ -2190,7 +2246,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>128</v>
       </c>
@@ -2207,7 +2263,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>130</v>
       </c>
@@ -2224,7 +2280,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>233</v>
       </c>
@@ -2241,7 +2297,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>242</v>
       </c>
@@ -2258,9 +2314,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2274,15 +2330,15 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2299,7 +2355,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2316,7 +2372,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>183</v>
       </c>
@@ -2333,7 +2389,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>186</v>
       </c>
@@ -2350,7 +2406,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2367,7 +2423,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2384,7 +2440,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>200</v>
       </c>
@@ -2401,7 +2457,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>202</v>
       </c>
@@ -2418,7 +2474,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
@@ -2435,7 +2491,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>77</v>
       </c>
@@ -2452,7 +2508,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>123</v>
       </c>
@@ -2469,7 +2525,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>205</v>
       </c>
@@ -2486,7 +2542,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>208</v>
       </c>
@@ -2503,7 +2559,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>216</v>
       </c>
@@ -2520,7 +2576,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>240</v>
       </c>
@@ -2537,7 +2593,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>248</v>
       </c>
@@ -2554,14 +2610,14 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2571,19 +2627,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2600,7 +2656,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2617,7 +2673,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2634,7 +2690,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>144</v>
       </c>
@@ -2651,26 +2707,26 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 1 SU and 1 DC
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\Career_Materials\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9F5E6E-295E-4114-A90B-D93146C6B83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEAC6AF-1D7E-4AF4-8946-FD944F8F47C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="615" windowWidth="24150" windowHeight="14985" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="10530" activeTab="3" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="308">
   <si>
     <t>Company Name</t>
   </si>
@@ -941,6 +941,30 @@
   </si>
   <si>
     <t>Christian Weedbrook</t>
+  </si>
+  <si>
+    <t>Arago</t>
+  </si>
+  <si>
+    <t>Si Photonics for AI acceleration (in stealth)</t>
+  </si>
+  <si>
+    <t>Hans-Christian Boos</t>
+  </si>
+  <si>
+    <t>Paris, France and San Francisco, California</t>
+  </si>
+  <si>
+    <t>Critical Frequency Design</t>
+  </si>
+  <si>
+    <t>Microwave photonics for communications and sensing. Frequency Specific Limiter via SBS. Free Space Optics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johnathen Warren and Charles Middleton </t>
+  </si>
+  <si>
+    <t>Melbourne, FL, USA</t>
   </si>
 </sst>
 </file>
@@ -1343,21 +1367,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="3" width="28.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="28.08203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="1"/>
+    <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1374,7 +1398,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1391,7 +1415,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1408,7 +1432,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1425,7 +1449,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1442,7 +1466,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -1459,7 +1483,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1476,7 +1500,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1493,7 +1517,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
@@ -1510,7 +1534,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1527,7 +1551,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1544,7 +1568,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1561,7 +1585,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1578,7 +1602,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1595,7 +1619,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1612,7 +1636,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
@@ -1629,7 +1653,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
@@ -1646,7 +1670,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
@@ -1663,7 +1687,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
@@ -1680,7 +1704,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
@@ -1697,7 +1721,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
         <v>97</v>
       </c>
@@ -1714,7 +1738,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="34" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
@@ -1731,7 +1755,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
@@ -1748,7 +1772,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
@@ -1765,7 +1789,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
@@ -1782,7 +1806,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
@@ -1799,7 +1823,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
         <v>120</v>
       </c>
@@ -1816,7 +1840,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
@@ -1833,7 +1857,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
@@ -1850,7 +1874,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
@@ -1867,7 +1891,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="3" t="s">
         <v>149</v>
       </c>
@@ -1884,7 +1908,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="1" t="s">
         <v>244</v>
       </c>
@@ -1901,7 +1925,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B34" s="1" t="s">
         <v>292</v>
       </c>
@@ -1918,7 +1942,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="1" t="s">
         <v>295</v>
       </c>
@@ -1935,7 +1959,23 @@
         <v>298</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="59.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C36" s="1">
+        <v>15</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1949,15 +1989,15 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1974,7 +2014,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
@@ -1991,7 +2031,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2008,7 +2048,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>257</v>
       </c>
@@ -2025,7 +2065,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -2042,7 +2082,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2059,7 +2099,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2076,7 +2116,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2093,7 +2133,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2110,7 +2150,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2127,7 +2167,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2144,7 +2184,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -2161,7 +2201,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>281</v>
       </c>
@@ -2178,7 +2218,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>286</v>
       </c>
@@ -2195,7 +2235,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>270</v>
       </c>
@@ -2212,7 +2252,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2229,7 +2269,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>102</v>
       </c>
@@ -2246,7 +2286,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>128</v>
       </c>
@@ -2263,7 +2303,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>130</v>
       </c>
@@ -2280,7 +2320,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="1" t="s">
         <v>233</v>
       </c>
@@ -2297,7 +2337,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
         <v>242</v>
       </c>
@@ -2314,9 +2354,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2330,15 +2370,15 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2355,7 +2395,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2372,7 +2412,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>183</v>
       </c>
@@ -2389,7 +2429,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>186</v>
       </c>
@@ -2406,7 +2446,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2423,7 +2463,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2440,7 +2480,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>200</v>
       </c>
@@ -2457,7 +2497,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>202</v>
       </c>
@@ -2474,7 +2514,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
@@ -2491,7 +2531,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>77</v>
       </c>
@@ -2508,7 +2548,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
         <v>123</v>
       </c>
@@ -2525,7 +2565,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>205</v>
       </c>
@@ -2542,7 +2582,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>208</v>
       </c>
@@ -2559,7 +2599,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>216</v>
       </c>
@@ -2576,7 +2616,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>240</v>
       </c>
@@ -2593,7 +2633,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
         <v>248</v>
       </c>
@@ -2610,14 +2650,14 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2627,19 +2667,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2656,7 +2696,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2673,7 +2713,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2690,7 +2730,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>144</v>
       </c>
@@ -2707,26 +2747,42 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C6" s="1">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 1 SU and 1 F
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEAC6AF-1D7E-4AF4-8946-FD944F8F47C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDB88E6-750F-41CE-9035-6794E42F27E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="10530" activeTab="3" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="16760" yWindow="0" windowWidth="19380" windowHeight="20880" activeTab="2" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="316">
   <si>
     <t>Company Name</t>
   </si>
@@ -965,13 +965,37 @@
   </si>
   <si>
     <t>Melbourne, FL, USA</t>
+  </si>
+  <si>
+    <t>Qphox</t>
+  </si>
+  <si>
+    <t>Delft, South Holland, Netherlands</t>
+  </si>
+  <si>
+    <t>Simon Groeblacher</t>
+  </si>
+  <si>
+    <t>By optically accessing qubits, our patented quantum transduction technology presents the first viable solution for scaling the performance of today’s most advanced quantum computers through connectivity and parallelization. https://www.nature.com/articles/s41565-023-01515-y</t>
+  </si>
+  <si>
+    <t>TSCM</t>
+  </si>
+  <si>
+    <t>Douglas Yu, Vice President of Pathfinding for System Integration</t>
+  </si>
+  <si>
+    <t>TSMC enters Si Ph layout out roadmap for 12.8 Tbps COUPE On-Package Interconnect</t>
+  </si>
+  <si>
+    <t>Hsinchu, Taiwan and Phoenix, Arizona, USA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -987,6 +1011,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -1014,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1029,6 +1061,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1365,24 +1400,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
-  <dimension ref="B1:F36"/>
+  <dimension ref="B1:F101"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="28.08203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.08203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
     <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1398,7 +1434,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1415,7 +1451,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1432,7 +1468,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1449,7 +1485,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1466,7 +1502,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -1483,7 +1519,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1500,7 +1536,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1517,7 +1553,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
@@ -1534,7 +1570,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1551,7 +1587,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1568,7 +1604,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1585,7 +1621,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1602,7 +1638,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1619,7 +1655,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1636,7 +1672,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
@@ -1653,7 +1689,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
@@ -1670,7 +1706,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
@@ -1687,7 +1723,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
@@ -1704,7 +1740,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
@@ -1721,7 +1757,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
         <v>97</v>
       </c>
@@ -1738,7 +1774,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="34" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
@@ -1755,7 +1791,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
@@ -1772,7 +1808,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
@@ -1789,7 +1825,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
@@ -1806,7 +1842,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
@@ -1823,7 +1859,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
         <v>120</v>
       </c>
@@ -1840,7 +1876,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
@@ -1857,7 +1893,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
@@ -1874,7 +1910,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
@@ -1891,7 +1927,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="3" t="s">
         <v>149</v>
       </c>
@@ -1908,8 +1944,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="1" t="s">
+    <row r="33" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="3" t="s">
         <v>244</v>
       </c>
       <c r="C33" s="1">
@@ -1925,8 +1961,8 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="1" t="s">
+    <row r="34" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B34" s="3" t="s">
         <v>292</v>
       </c>
       <c r="C34" s="1">
@@ -1942,8 +1978,8 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="1" t="s">
+    <row r="35" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="3" t="s">
         <v>295</v>
       </c>
       <c r="C35" s="1">
@@ -1959,8 +1995,8 @@
         <v>298</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="1" t="s">
+    <row r="36" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="3" t="s">
         <v>300</v>
       </c>
       <c r="C36" s="1">
@@ -1976,6 +2012,87 @@
         <v>303</v>
       </c>
     </row>
+    <row r="37" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C37" s="1">
+        <v>40</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="39" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="41" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="42" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="44" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="45" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="2:6" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="51" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="54" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="55" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="57" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="58" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="60" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="61" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="64" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="65" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="67" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="70" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="71" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="73" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="74" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="77" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="78" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="79" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="80" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="81" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="82" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="83" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="84" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="85" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="86" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="87" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="88" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="89" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="90" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="91" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="92" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="93" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="94" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="95" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="96" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="97" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="98" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="99" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="100" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="101" ht="56" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2366,8 +2483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3E1C2-3C44-2549-B6BE-21FD6EE1DD33}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -2650,7 +2767,23 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F18" t="s">
+        <v>315</v>
+      </c>
+    </row>
     <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="21" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2667,8 +2800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Added 1 LC, also added cache and rewrote get_coords functions to vastly speed up regenerating map from 2-3 mins to < 10 seconds. New locations which still take about 10 seconds each but then be saved to chache.
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\Career_Materials\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9EB0FE-92CC-40AC-8223-00E1CD807319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42883167-B09E-4036-A9EA-B7A824080272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="615" windowWidth="24150" windowHeight="14985" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="324">
   <si>
     <t>Company Name</t>
   </si>
@@ -801,9 +801,6 @@
     <t>Palo Alto, California and Grenoble, France</t>
   </si>
   <si>
-    <t>CTO Tolga Kurtoglu</t>
-  </si>
-  <si>
     <t>Design Software and Assistance for photonic integrated circuits, OptoDesigner</t>
   </si>
   <si>
@@ -1001,6 +998,22 @@
   </si>
   <si>
     <t>Leeds, England and Bristol, England</t>
+  </si>
+  <si>
+    <t>Microsoft Research</t>
+  </si>
+  <si>
+    <t>Analog Optical Computing. MicroLed Array, Free Space MVM, Electrical Nonlinearity</t>
+  </si>
+  <si>
+    <t>H. Ballani, G. Brennan, B. Canakci, J. Chu, J. H. Clegg, D. Cletheroe, C. Gkantsidis, J. Gladrow, K. P.
+Kalinin, D. J. Kelly, H. Kremer, G. O'Shea, F. Parmigiani, L. Pickup, B. Rahmani, A. Rowstron</t>
+  </si>
+  <si>
+    <t>Cambridge, England</t>
+  </si>
+  <si>
+    <t>CTO Tolga Kurtoglu; Fabian Böhm,, Bassem Tossoun, Thomas Van Vaerenbergh</t>
   </si>
 </sst>
 </file>
@@ -1414,22 +1427,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="2" width="28.125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="28.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="28.08203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.08203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="1"/>
+    <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1459,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1463,7 +1476,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1480,7 +1493,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1497,7 +1510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1514,7 +1527,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -1531,7 +1544,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1548,7 +1561,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1565,7 +1578,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
@@ -1582,7 +1595,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1599,7 +1612,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1616,7 +1629,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1633,7 +1646,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1650,7 +1663,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1667,7 +1680,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1684,7 +1697,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
@@ -1701,7 +1714,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
@@ -1718,7 +1731,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
@@ -1735,7 +1748,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
@@ -1752,7 +1765,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
@@ -1769,7 +1782,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
         <v>97</v>
       </c>
@@ -1786,7 +1799,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
@@ -1803,7 +1816,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
@@ -1820,7 +1833,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
@@ -1837,7 +1850,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
@@ -1854,7 +1867,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
@@ -1871,7 +1884,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
         <v>120</v>
       </c>
@@ -1888,7 +1901,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
@@ -1905,7 +1918,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
@@ -1922,7 +1935,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
@@ -1939,7 +1952,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="3" t="s">
         <v>149</v>
       </c>
@@ -1956,7 +1969,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="3" t="s">
         <v>244</v>
       </c>
@@ -1973,154 +1986,154 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C34" s="1">
         <v>190</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F34" s="1" t="s">
+    </row>
+    <row r="35" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="3" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="3" t="s">
-        <v>295</v>
       </c>
       <c r="C35" s="1">
         <v>30</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C36" s="1">
         <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C37" s="1">
         <v>40</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C38" s="1">
         <v>30</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="39" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="41" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="42" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="44" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="45" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="51" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="54" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="55" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="57" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="58" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="60" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="61" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="64" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="65" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="67" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="70" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="71" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="73" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="74" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="77" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="78" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="79" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="80" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="81" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="82" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="83" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="84" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="85" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="86" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="87" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="88" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="89" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="90" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="91" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="92" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="93" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="94" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="95" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="96" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="97" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="98" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="99" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="100" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="101" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2131,19 +2144,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2160,7 +2173,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
@@ -2177,7 +2190,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2194,9 +2207,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C5" s="1">
         <v>500</v>
@@ -2208,10 +2221,10 @@
         <v>173</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -2228,7 +2241,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2245,7 +2258,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2262,7 +2275,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2279,7 +2292,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2290,13 +2303,13 @@
         <v>237</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2304,16 +2317,16 @@
         <v>8000</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2321,16 +2334,16 @@
         <v>150</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -2338,67 +2351,67 @@
         <v>700</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E13" s="1" t="s">
+    </row>
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="C14" s="1">
         <v>800</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C15" s="5">
         <v>1400</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C16" s="1">
         <v>500</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2406,16 +2419,16 @@
         <v>100</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>102</v>
       </c>
@@ -2423,16 +2436,16 @@
         <v>30</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>128</v>
       </c>
@@ -2440,16 +2453,16 @@
         <v>15000</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>130</v>
       </c>
@@ -2457,16 +2470,16 @@
         <v>14000</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="1" t="s">
         <v>233</v>
       </c>
@@ -2483,7 +2496,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
         <v>242</v>
       </c>
@@ -2494,15 +2507,31 @@
         <v>243</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>253</v>
+        <v>323</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C23" s="1">
+        <v>100</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2516,15 +2545,15 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2541,7 +2570,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2558,7 +2587,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>183</v>
       </c>
@@ -2575,7 +2604,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>186</v>
       </c>
@@ -2592,7 +2621,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2609,7 +2638,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2626,7 +2655,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>200</v>
       </c>
@@ -2643,7 +2672,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>202</v>
       </c>
@@ -2660,7 +2689,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
@@ -2677,7 +2706,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>77</v>
       </c>
@@ -2694,7 +2723,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
         <v>123</v>
       </c>
@@ -2708,10 +2737,10 @@
         <v>214</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>205</v>
       </c>
@@ -2728,7 +2757,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>208</v>
       </c>
@@ -2742,10 +2771,10 @@
         <v>220</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>216</v>
       </c>
@@ -2762,7 +2791,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>240</v>
       </c>
@@ -2779,7 +2808,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
         <v>248</v>
       </c>
@@ -2796,30 +2825,30 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C18" s="1">
         <v>1000</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F18" t="s">
         <v>314</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F18" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2833,15 +2862,15 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2858,7 +2887,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2875,7 +2904,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2892,7 +2921,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>144</v>
       </c>
@@ -2909,42 +2938,42 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C6" s="1">
         <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added function to check if coords are over water, Link commented about the startup which was headquatered within the hudson, we can't have that
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\Career_Materials\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42883167-B09E-4036-A9EA-B7A824080272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722E1D73-C096-4BA3-A81E-D5977E01EB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="0" yWindow="615" windowWidth="24150" windowHeight="14985" activeTab="1" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -1431,18 +1431,18 @@
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="28.08203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="28.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="28.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="28.125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>97</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>120</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>149</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>244</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>291</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>294</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>299</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>307</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>315</v>
       </c>
@@ -2071,69 +2071,69 @@
         <v>318</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="40" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="41" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="42" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="43" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="45" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="46" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="47" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="48" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="49" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="50" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="51" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="52" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="53" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="54" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="55" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="56" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="57" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="58" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="59" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="60" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="61" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="62" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="63" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="64" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="65" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="66" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="67" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="68" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="69" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="70" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="71" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="72" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="73" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="74" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="77" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="78" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="79" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="82" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="85" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="86" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="89" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="91" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="92" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="93" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="94" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="95" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="96" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="97" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="99" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="100" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="101" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="39" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2144,19 +2144,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>256</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>280</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>285</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>269</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>102</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>128</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>130</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>233</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>242</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>319</v>
       </c>
@@ -2530,8 +2530,8 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2545,15 +2545,15 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>183</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>186</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>200</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>202</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>77</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>123</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>205</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>208</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>216</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>240</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>248</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>311</v>
       </c>
@@ -2842,13 +2842,13 @@
         <v>314</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:6" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2862,15 +2862,15 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>144</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>303</v>
       </c>
@@ -2955,25 +2955,25 @@
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 2 LC, and 1 F
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\Career_Materials\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722E1D73-C096-4BA3-A81E-D5977E01EB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177830D7-8414-4143-9E5C-C5B02749F33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="615" windowWidth="24150" windowHeight="14985" activeTab="1" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="334">
   <si>
     <t>Company Name</t>
   </si>
@@ -1014,13 +1014,43 @@
   </si>
   <si>
     <t>CTO Tolga Kurtoglu; Fabian Böhm,, Bassem Tossoun, Thomas Van Vaerenbergh</t>
+  </si>
+  <si>
+    <t>"WaveFabric", switches, transceivers, silicon photonics</t>
+  </si>
+  <si>
+    <t>Nokia</t>
+  </si>
+  <si>
+    <t>Nokia Bell Labs</t>
+  </si>
+  <si>
+    <t>Neuromophic Photonics, Integrated photonics research, compute</t>
+  </si>
+  <si>
+    <t>President: Peter Vetter, Researchers: Mohamad Hossein Idjadi</t>
+  </si>
+  <si>
+    <t>Murray Hill, NJ, USA and New Brunswick, New Jersey</t>
+  </si>
+  <si>
+    <t>Marc Ulrich</t>
+  </si>
+  <si>
+    <t>Aluvia Photonics</t>
+  </si>
+  <si>
+    <t>MPW Runs Al2O3 integrated photonic platform; 200nm-3microns; rare-earth doping amplifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve Stoffels and Michiel de Goede, University of Twente </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1050,6 +1080,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF474747"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1071,7 +1115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1089,6 +1133,24 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1428,7 +1490,7 @@
   <dimension ref="B1:F101"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -2144,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2530,8 +2592,40 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C24" s="1">
+        <v>500</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C25" s="1">
+        <v>200</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2541,308 +2635,325 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3E1C2-3C44-2549-B6BE-21FD6EE1DD33}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="2" max="6" width="28.125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="28.125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:6" s="12" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="12" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="11">
         <v>13000</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="7">
         <v>500</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="7" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="7">
         <v>130</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="7" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="7" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="7" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="7">
         <v>70</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="7" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="11">
         <v>10000</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="7">
         <v>100</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="7" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="7" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="11">
         <v>5500</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="7" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="11">
         <v>4500</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="7" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="7">
         <v>20</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="7" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="7">
         <v>20</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="7" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="7">
         <v>150</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="7" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="7">
         <v>1000</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="8" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C19" s="7">
+        <v>20</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
     <row r="20" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added 11 new companies
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\Career_Materials\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177830D7-8414-4143-9E5C-C5B02749F33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61137B5-747F-42AF-9851-A8A48265ED82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="374">
   <si>
     <t>Company Name</t>
   </si>
@@ -1044,6 +1044,127 @@
   </si>
   <si>
     <t xml:space="preserve">Steve Stoffels and Michiel de Goede, University of Twente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thin Film Lithium Niobate, telecom/datacom. Applications: Quantum, Reservoir, Remote Sensing, Quan. Crypt. </t>
+  </si>
+  <si>
+    <t>CEO William McGann, CTO Yong Meng Sua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantum Comptuing, Inc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tempe, Arizona, USA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoboken, New Jersey, USA </t>
+  </si>
+  <si>
+    <t>Maynard, Massachusetts, USA</t>
+  </si>
+  <si>
+    <t>Optical Networking, Small Form Factor Pluggable Tranceivers</t>
+  </si>
+  <si>
+    <t>Acacia Communications</t>
+  </si>
+  <si>
+    <t>CEO: Raj Shanmugaraj , CTO:Benny P. Mikkelsen</t>
+  </si>
+  <si>
+    <t>APIC Corporation</t>
+  </si>
+  <si>
+    <t>Chip-scale optical networks for energy-efficient high performance computing (HPC). High dynamic range links</t>
+  </si>
+  <si>
+    <t>Culver City, CA</t>
+  </si>
+  <si>
+    <t>CEO/CTO: Birendra Dutt, VP of Optics: Koichi Sayano, VP of SiPh Ashok K. Kapoor</t>
+  </si>
+  <si>
+    <t>Pilot Photonics</t>
+  </si>
+  <si>
+    <t>Glasnevin, Dublin, Ireland</t>
+  </si>
+  <si>
+    <t>single-chip photonic integrated circuits with comb-enhanced capabilities. Lidar</t>
+  </si>
+  <si>
+    <t>CEO: William Oppermann, CTO: Dr. Frank Smyth</t>
+  </si>
+  <si>
+    <t>RANOVUS Inc.</t>
+  </si>
+  <si>
+    <t>Quantum Dot Multi-Wavelength Laser, Optical Interconnects, PICs</t>
+  </si>
+  <si>
+    <t>Ottawa, Ontario, Canada</t>
+  </si>
+  <si>
+    <t>CEO: Hamid Arabzadeh and VP of Opt.:Doug Beckett</t>
+  </si>
+  <si>
+    <t>Cailabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Space Telecommunications, Integrated Photonic solutions, </t>
+  </si>
+  <si>
+    <t>Rennes, Bretagne, France and Washington, USA</t>
+  </si>
+  <si>
+    <t>CEO: Pu Jian</t>
+  </si>
+  <si>
+    <t>Analog Photonics</t>
+  </si>
+  <si>
+    <t>LiDAR. Telecommunications, free-space optical communications, and  Silicon PICs</t>
+  </si>
+  <si>
+    <t>CEO: Michael Watts, MIT</t>
+  </si>
+  <si>
+    <t>Boston, MA, USA</t>
+  </si>
+  <si>
+    <t>HyperLight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFLN, 100 GHz, 1dB loss, 1V drive, Transmitters, </t>
+  </si>
+  <si>
+    <t>CEO: Mian Zhang, Harvard University</t>
+  </si>
+  <si>
+    <t>Cambridge, Massachusetts, USA</t>
+  </si>
+  <si>
+    <t>SiPhotonIC Technologies</t>
+  </si>
+  <si>
+    <t>Rapid &amp; high-precision prototyping of Silicon Photonic Integrated Circuits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEO: Yunhong Ding
+ </t>
+  </si>
+  <si>
+    <t>Alcyon Photonics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEO: Jimena Garcia-Romeu, Photonics Design Lead: Dr. Irene Olivares </t>
+  </si>
+  <si>
+    <t>Alcyon Photonics foundry validated library of Photonics Integrated Circuits, SiPh and IIIV</t>
+  </si>
+  <si>
+    <t>Madrid, Spain</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1152,6 +1273,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1489,22 +1613,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F101"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="2" width="28.125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="28.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="28.08203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.08203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="1"/>
+    <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1521,7 +1645,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1538,7 +1662,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1555,7 +1679,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1572,7 +1696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1589,7 +1713,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -1606,7 +1730,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1623,7 +1747,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1640,7 +1764,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
@@ -1657,7 +1781,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1674,7 +1798,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1691,7 +1815,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1708,7 +1832,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1725,7 +1849,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1742,7 +1866,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1759,7 +1883,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
@@ -1776,7 +1900,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
@@ -1793,7 +1917,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
@@ -1810,7 +1934,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
@@ -1827,7 +1951,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
@@ -1844,7 +1968,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
         <v>97</v>
       </c>
@@ -1861,7 +1985,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
@@ -1878,7 +2002,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
@@ -1895,7 +2019,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
@@ -1912,7 +2036,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
@@ -1929,7 +2053,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
@@ -1946,7 +2070,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
         <v>120</v>
       </c>
@@ -1963,7 +2087,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
@@ -1980,7 +2104,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
@@ -1997,7 +2121,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
@@ -2014,7 +2138,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="3" t="s">
         <v>149</v>
       </c>
@@ -2031,7 +2155,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="3" t="s">
         <v>244</v>
       </c>
@@ -2048,7 +2172,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="3" t="s">
         <v>291</v>
       </c>
@@ -2065,7 +2189,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="3" t="s">
         <v>294</v>
       </c>
@@ -2082,7 +2206,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="3" t="s">
         <v>299</v>
       </c>
@@ -2099,7 +2223,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="3" t="s">
         <v>307</v>
       </c>
@@ -2116,7 +2240,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" s="3" t="s">
         <v>315</v>
       </c>
@@ -2133,69 +2257,197 @@
         <v>318</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C39" s="7">
+        <v>50</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C40" s="1">
+        <v>20</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C41" s="1">
+        <v>81</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C42" s="1">
+        <v>120</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C43" s="1">
+        <v>20</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C44" s="1">
+        <v>50</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C45" s="1">
+        <v>10</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C46" s="1">
+        <v>20</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="51" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="54" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="55" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="57" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="58" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="60" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="61" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="64" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="65" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="67" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="70" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="71" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="73" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="74" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="77" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="78" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="79" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="80" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="81" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="82" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="83" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="84" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="85" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="86" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="87" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="88" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="89" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="90" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="91" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="92" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="93" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="94" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="95" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="96" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="97" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="98" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="99" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="100" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="101" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2204,21 +2456,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
-  <dimension ref="B1:F25"/>
+  <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2235,7 +2487,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
@@ -2252,7 +2504,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2269,7 +2521,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>256</v>
       </c>
@@ -2286,7 +2538,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -2303,7 +2555,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2320,7 +2572,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2337,7 +2589,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2354,7 +2606,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2371,7 +2623,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2388,7 +2640,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2405,7 +2657,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -2422,7 +2674,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>280</v>
       </c>
@@ -2439,7 +2691,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>285</v>
       </c>
@@ -2456,7 +2708,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>269</v>
       </c>
@@ -2473,7 +2725,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2490,7 +2742,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>102</v>
       </c>
@@ -2507,7 +2759,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>128</v>
       </c>
@@ -2524,7 +2776,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>130</v>
       </c>
@@ -2541,7 +2793,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="1" t="s">
         <v>233</v>
       </c>
@@ -2558,7 +2810,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
         <v>242</v>
       </c>
@@ -2575,7 +2827,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="1" t="s">
         <v>319</v>
       </c>
@@ -2592,7 +2844,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
         <v>325</v>
       </c>
@@ -2609,7 +2861,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="1" t="s">
         <v>326</v>
       </c>
@@ -2626,6 +2878,42 @@
         <v>329</v>
       </c>
     </row>
+    <row r="26" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C26" s="1">
+        <v>400</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="29" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="30" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="32" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="33" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="37" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="38" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="39" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="40" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="43" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="44" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="45" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2633,22 +2921,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3E1C2-3C44-2549-B6BE-21FD6EE1DD33}">
-  <dimension ref="B1:F25"/>
+  <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="6" width="28.125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="6" width="28.08203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" s="12" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" s="12" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
@@ -2665,7 +2953,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="7" t="s">
         <v>23</v>
       </c>
@@ -2682,7 +2970,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>183</v>
       </c>
@@ -2699,7 +2987,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>186</v>
       </c>
@@ -2716,7 +3004,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="7" t="s">
         <v>24</v>
       </c>
@@ -2733,7 +3021,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
@@ -2750,7 +3038,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="s">
         <v>200</v>
       </c>
@@ -2767,7 +3055,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="7" t="s">
         <v>202</v>
       </c>
@@ -2784,7 +3072,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="s">
         <v>61</v>
       </c>
@@ -2801,7 +3089,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="s">
         <v>77</v>
       </c>
@@ -2818,7 +3106,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>123</v>
       </c>
@@ -2835,7 +3123,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="s">
         <v>205</v>
       </c>
@@ -2852,7 +3140,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="s">
         <v>208</v>
       </c>
@@ -2869,7 +3157,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="s">
         <v>216</v>
       </c>
@@ -2886,7 +3174,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="7" t="s">
         <v>240</v>
       </c>
@@ -2903,7 +3191,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="7" t="s">
         <v>248</v>
       </c>
@@ -2920,7 +3208,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="7" t="s">
         <v>311</v>
       </c>
@@ -2937,7 +3225,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="7" t="s">
         <v>331</v>
       </c>
@@ -2954,12 +3242,29 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C20" s="7">
+        <v>50</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="26" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2969,19 +3274,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2998,7 +3303,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -3015,7 +3320,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -3032,7 +3337,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>144</v>
       </c>
@@ -3049,7 +3354,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>303</v>
       </c>
@@ -3066,25 +3371,41 @@
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C7" s="1">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding 1 SU, 1 DC
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\GitHub\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61137B5-747F-42AF-9851-A8A48265ED82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36412ED-C6CE-47B7-9784-95286AEACE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="382">
   <si>
     <t>Company Name</t>
   </si>
@@ -1165,6 +1165,30 @@
   </si>
   <si>
     <t>Madrid, Spain</t>
+  </si>
+  <si>
+    <t>Teramount</t>
+  </si>
+  <si>
+    <t>Silicon Photonic Transceivers and Switches, Chip-to-Chip Interconnects, SiPh Sensors, 5G/6G Networks: Photonic Couplers</t>
+  </si>
+  <si>
+    <t>CEO: Hesham Taha, CTO: Avi Israel</t>
+  </si>
+  <si>
+    <t>Jerusalem, Israel</t>
+  </si>
+  <si>
+    <t>Physical Sciences Inc</t>
+  </si>
+  <si>
+    <t>CEO: Bill Marinelli, VP Photonics: Joel Hensley</t>
+  </si>
+  <si>
+    <t>Andover, Massachusetts and Wilmington, Massachusetts and Pleasanton, California</t>
+  </si>
+  <si>
+    <t>Quantum information, RF photonics, Optical communication, LiDAR, Integrated Photonics</t>
   </si>
 </sst>
 </file>
@@ -1613,22 +1637,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView topLeftCell="B41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="28.08203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="28.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="28.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="28.125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1645,7 +1669,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1662,7 +1686,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1679,7 +1703,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1696,7 +1720,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1713,7 +1737,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -1730,7 +1754,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1747,7 +1771,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1764,7 +1788,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
@@ -1781,7 +1805,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
@@ -1798,7 +1822,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1815,7 +1839,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1832,7 +1856,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1849,7 +1873,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -1866,7 +1890,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1883,7 +1907,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
@@ -1900,7 +1924,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
@@ -1917,7 +1941,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
@@ -1934,7 +1958,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
@@ -1951,7 +1975,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
@@ -1968,7 +1992,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>97</v>
       </c>
@@ -1985,7 +2009,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
@@ -2002,7 +2026,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
@@ -2019,7 +2043,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
@@ -2036,7 +2060,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
@@ -2053,7 +2077,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
@@ -2070,7 +2094,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>120</v>
       </c>
@@ -2087,7 +2111,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
@@ -2104,7 +2128,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
@@ -2121,7 +2145,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
@@ -2138,7 +2162,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>149</v>
       </c>
@@ -2155,7 +2179,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>244</v>
       </c>
@@ -2172,7 +2196,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>291</v>
       </c>
@@ -2189,7 +2213,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>294</v>
       </c>
@@ -2206,7 +2230,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>299</v>
       </c>
@@ -2223,7 +2247,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>307</v>
       </c>
@@ -2240,7 +2264,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>315</v>
       </c>
@@ -2257,7 +2281,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="13" t="s">
         <v>336</v>
       </c>
@@ -2274,7 +2298,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
         <v>347</v>
       </c>
@@ -2291,7 +2315,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
         <v>351</v>
       </c>
@@ -2308,7 +2332,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
         <v>355</v>
       </c>
@@ -2325,7 +2349,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>359</v>
       </c>
@@ -2342,7 +2366,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
         <v>363</v>
       </c>
@@ -2359,7 +2383,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="3" t="s">
         <v>367</v>
       </c>
@@ -2376,7 +2400,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>370</v>
       </c>
@@ -2393,61 +2417,77 @@
         <v>373</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="48" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="49" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="50" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="51" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="52" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="53" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="54" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="55" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="56" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="57" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="58" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="59" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="60" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="61" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="62" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="63" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="64" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="65" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="66" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="67" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="68" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="69" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="70" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="71" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="72" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="73" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="74" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="77" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="78" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="79" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="82" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="85" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="86" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="89" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="91" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="92" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="93" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="94" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="95" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="96" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="97" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="99" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="100" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="101" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C47" s="1">
+        <v>50</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2462,15 +2502,15 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2487,7 +2527,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
@@ -2504,7 +2544,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2521,7 +2561,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>256</v>
       </c>
@@ -2538,7 +2578,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -2555,7 +2595,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2572,7 +2612,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2589,7 +2629,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2606,7 +2646,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2623,7 +2663,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2640,7 +2680,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2657,7 +2697,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -2674,7 +2714,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>280</v>
       </c>
@@ -2691,7 +2731,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>285</v>
       </c>
@@ -2708,7 +2748,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>269</v>
       </c>
@@ -2725,7 +2765,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2742,7 +2782,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>102</v>
       </c>
@@ -2759,7 +2799,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>128</v>
       </c>
@@ -2776,7 +2816,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>130</v>
       </c>
@@ -2793,7 +2833,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>233</v>
       </c>
@@ -2810,7 +2850,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>242</v>
       </c>
@@ -2827,7 +2867,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>319</v>
       </c>
@@ -2844,7 +2884,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>325</v>
       </c>
@@ -2861,7 +2901,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>326</v>
       </c>
@@ -2878,7 +2918,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>341</v>
       </c>
@@ -2895,25 +2935,25 @@
         <v>339</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="28" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="29" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="30" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="31" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="32" spans="2:6" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="33" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" ht="59" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2927,16 +2967,16 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="6" width="28.08203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="6" width="28.125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" s="12" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" s="12" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
@@ -2953,7 +2993,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>23</v>
       </c>
@@ -2970,7 +3010,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>183</v>
       </c>
@@ -2987,7 +3027,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>186</v>
       </c>
@@ -3004,7 +3044,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>24</v>
       </c>
@@ -3021,7 +3061,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
@@ -3038,7 +3078,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>200</v>
       </c>
@@ -3055,7 +3095,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>202</v>
       </c>
@@ -3072,7 +3112,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>61</v>
       </c>
@@ -3089,7 +3129,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>77</v>
       </c>
@@ -3106,7 +3146,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>123</v>
       </c>
@@ -3123,7 +3163,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>205</v>
       </c>
@@ -3140,7 +3180,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>208</v>
       </c>
@@ -3157,7 +3197,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>216</v>
       </c>
@@ -3174,7 +3214,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>240</v>
       </c>
@@ -3191,7 +3231,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>248</v>
       </c>
@@ -3208,7 +3248,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>311</v>
       </c>
@@ -3225,7 +3265,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>331</v>
       </c>
@@ -3242,7 +3282,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>336</v>
       </c>
@@ -3259,12 +3299,12 @@
         <v>337</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="26" spans="2:6" ht="56.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:6" ht="56.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3274,19 +3314,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3303,7 +3343,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -3320,7 +3360,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -3337,7 +3377,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>144</v>
       </c>
@@ -3354,7 +3394,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>303</v>
       </c>
@@ -3371,7 +3411,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>343</v>
       </c>
@@ -3388,24 +3428,40 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C8" s="1">
+        <v>300</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 1 SU, 1 LC
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\GitHub\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA271ECD-047E-40B8-B2A7-53A11DC48872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B034D3-3648-4939-A2D8-F45C3CDF72E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="395">
   <si>
     <t>Company Name</t>
   </si>
@@ -1201,6 +1201,33 @@
   </si>
   <si>
     <t>EFFECT Photonics</t>
+  </si>
+  <si>
+    <t>NASA Jet Propulsion Laboratory (JPL)</t>
+  </si>
+  <si>
+    <t> Pasadena, California, USA</t>
+  </si>
+  <si>
+    <t>Chip-scale stable lasers using MEMS and nanophotonic technologies, SiN, LiNo, Hetero, Sensors, PIC-based coronagraph instrument</t>
+  </si>
+  <si>
+    <t>Amanda N. Bozovich</t>
+  </si>
+  <si>
+    <t>Look Dynamics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 10 </t>
+  </si>
+  <si>
+    <t>Longmont, Colorado</t>
+  </si>
+  <si>
+    <t>Photonic Convolutional Neural Networks, Integrated, Diffractive Optics, https://lookdynamics.com/</t>
+  </si>
+  <si>
+    <t>Rikki J. Crill, Jonathan C. Baiardo, David A. Bruce</t>
   </si>
 </sst>
 </file>
@@ -1650,7 +1677,7 @@
   <dimension ref="B1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -2463,22 +2490,38 @@
         <v>382</v>
       </c>
     </row>
-    <row r="49" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2526,8 +2569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A18" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2963,7 +3006,23 @@
         <v>339</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C27" s="1">
+        <v>500</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
     <row r="28" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added 1 SU, 1 F
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecb10\Desktop\GitHub\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79D14E3-FA8A-45BE-95CF-CB7E7CF0A0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0326F921-F38F-4DC2-B7DA-68BCFB3B9DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="442">
   <si>
     <t>Company Name</t>
   </si>
@@ -1354,6 +1354,22 @@
   </si>
   <si>
     <t>CEO: Jim Somers, COO: Chris Herbert</t>
+  </si>
+  <si>
+    <t>Goleta, California</t>
+  </si>
+  <si>
+    <t>Freedom Photonics</t>
+  </si>
+  <si>
+    <t>Tunable Lasers, Custom PICs, Photodetectors, Switches, Optical Delay Lines. InP, GaAs, Si-Ge, Si Photonics, Aquired by Luminar (2022)</t>
+  </si>
+  <si>
+    <t>CEO: Dr. Milan L. Mashanovitch, Dr. Leif A. Johansson, Dr. Gordon B. Morrison</t>
+  </si>
+  <si>
+    <t>InP, GaAs, Si-Ge, Si Photonics. 
+Photonic Device Design, Photonic Chip Fabrication, Photonic Chip Fabrication, Packaging, Wirebonding (electrical and photonic), Subsystem Design,   Aquired by Luminar (2022)</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1414,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -1425,7 +1441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1457,13 +1473,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1802,26 +1815,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F100"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D49" sqref="B49:D49"/>
+    <sheetView topLeftCell="B41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F49" sqref="B49:F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="28.08203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="28.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="3" width="28.125" style="3" customWidth="1"/>
     <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="28.125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1834,11 +1846,11 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>200</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1851,11 +1863,11 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>200</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1868,11 +1880,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1885,11 +1897,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>280</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1902,11 +1914,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1919,11 +1931,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>100</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1936,11 +1948,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1953,11 +1965,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1970,11 +1982,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1987,11 +1999,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2004,11 +2016,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2021,11 +2033,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -2038,11 +2050,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2055,11 +2067,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -2072,11 +2084,11 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -2089,11 +2101,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -2106,11 +2118,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -2123,11 +2135,11 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -2140,11 +2152,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -2157,11 +2169,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="3">
         <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -2174,11 +2186,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="3" t="s">
         <v>105</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -2191,11 +2203,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="3" t="s">
         <v>108</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -2208,11 +2220,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -2225,11 +2237,11 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -2242,11 +2254,11 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -2259,11 +2271,11 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -2276,11 +2288,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="3" t="s">
         <v>125</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -2293,11 +2305,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -2310,11 +2322,11 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -2327,11 +2339,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>137</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -2344,11 +2356,11 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="3">
         <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -2361,11 +2373,11 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="3">
         <v>190</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -2378,11 +2390,11 @@
         <v>293</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="3">
         <v>30</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -2395,11 +2407,11 @@
         <v>297</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="3">
         <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -2412,11 +2424,11 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="3">
         <v>40</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -2429,11 +2441,11 @@
         <v>308</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="3">
         <v>30</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -2446,11 +2458,11 @@
         <v>318</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="12" t="s">
+    <row r="39" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
         <v>336</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="11">
         <v>50</v>
       </c>
       <c r="D39" s="7" t="s">
@@ -2463,11 +2475,11 @@
         <v>338</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="3">
         <v>20</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -2480,11 +2492,11 @@
         <v>348</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="3">
         <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -2497,11 +2509,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="3">
         <v>120</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -2514,11 +2526,11 @@
         <v>357</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="3">
         <v>20</v>
       </c>
       <c r="D43" s="1" t="s">
@@ -2531,11 +2543,11 @@
         <v>362</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="3">
         <v>50</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2548,11 +2560,11 @@
         <v>366</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="3">
         <v>20</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2565,11 +2577,11 @@
         <v>373</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="3">
         <v>50</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -2582,11 +2594,11 @@
         <v>377</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="3">
         <v>150</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2599,12 +2611,12 @@
         <v>382</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>391</v>
+      <c r="C48" s="3">
+        <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>393</v>
@@ -2616,60 +2628,74 @@
         <v>392</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="51" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="52" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="53" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="54" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="55" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="56" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="57" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="58" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="59" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="60" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="61" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="62" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="63" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="64" spans="2:2" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="65" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="66" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="67" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="68" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="69" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="70" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="71" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="72" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="73" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="74" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="77" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="78" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="79" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="82" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="85" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="86" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="89" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="91" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="92" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="93" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="94" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="95" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="96" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="97" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="99" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="100" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C49" s="3">
+        <v>104</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="56.1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2684,15 +2710,15 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2709,7 +2735,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>162</v>
       </c>
@@ -2726,7 +2752,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2743,7 +2769,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>256</v>
       </c>
@@ -2760,7 +2786,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -2777,7 +2803,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2794,7 +2820,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2811,7 +2837,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2828,7 +2854,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2845,7 +2871,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2862,7 +2888,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2879,7 +2905,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -2896,7 +2922,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>280</v>
       </c>
@@ -2913,7 +2939,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>285</v>
       </c>
@@ -2930,7 +2956,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>269</v>
       </c>
@@ -2947,7 +2973,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -2964,7 +2990,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>102</v>
       </c>
@@ -2981,7 +3007,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>128</v>
       </c>
@@ -2998,7 +3024,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>130</v>
       </c>
@@ -3015,7 +3041,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>233</v>
       </c>
@@ -3032,7 +3058,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>242</v>
       </c>
@@ -3049,7 +3075,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>319</v>
       </c>
@@ -3066,7 +3092,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>325</v>
       </c>
@@ -3083,7 +3109,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>326</v>
       </c>
@@ -3100,7 +3126,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>341</v>
       </c>
@@ -3117,7 +3143,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>386</v>
       </c>
@@ -3134,24 +3160,24 @@
         <v>387</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="29" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="30" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="31" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="32" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="33" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:6" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="59.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3161,40 +3187,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3E1C2-3C44-2549-B6BE-21FD6EE1DD33}">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="28.08203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="28.08203125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="28.08203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="3" width="28.125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="28.125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" s="11" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="11" t="s">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" s="12" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="5">
@@ -3210,8 +3235,8 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>183</v>
       </c>
       <c r="C4" s="1">
@@ -3227,8 +3252,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>186</v>
       </c>
       <c r="C5" s="1">
@@ -3244,8 +3269,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -3261,8 +3286,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -3278,8 +3303,8 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>200</v>
       </c>
       <c r="C8" s="1">
@@ -3295,8 +3320,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>202</v>
       </c>
       <c r="C9" s="5">
@@ -3312,8 +3337,8 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C10" s="1">
@@ -3329,8 +3354,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -3346,8 +3371,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="13" t="s">
+    <row r="12" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C12" s="5">
@@ -3363,8 +3388,8 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>205</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -3380,8 +3405,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="13" t="s">
+    <row r="14" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>208</v>
       </c>
       <c r="C14" s="5">
@@ -3397,8 +3422,8 @@
         <v>289</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="13" t="s">
+    <row r="15" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C15" s="1">
@@ -3414,8 +3439,8 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>240</v>
       </c>
       <c r="C16" s="1">
@@ -3431,8 +3456,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C17" s="1">
@@ -3448,8 +3473,8 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="13" t="s">
+    <row r="18" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>311</v>
       </c>
       <c r="C18" s="1">
@@ -3465,8 +3490,8 @@
         <v>314</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="13" t="s">
+    <row r="19" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>331</v>
       </c>
       <c r="C19" s="1">
@@ -3482,8 +3507,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="13" t="s">
+    <row r="20" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>336</v>
       </c>
       <c r="C20" s="1">
@@ -3499,8 +3524,8 @@
         <v>337</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="13" t="s">
+    <row r="21" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>396</v>
       </c>
       <c r="C21" s="1">
@@ -3516,8 +3541,8 @@
         <v>397</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="13" t="s">
+    <row r="22" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>399</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -3533,8 +3558,8 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="13" t="s">
+    <row r="23" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>403</v>
       </c>
       <c r="C23" s="1">
@@ -3550,8 +3575,8 @@
         <v>405</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="13" t="s">
+    <row r="24" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>367</v>
       </c>
       <c r="C24" s="1">
@@ -3567,8 +3592,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="13" t="s">
+    <row r="25" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>406</v>
       </c>
       <c r="C25" s="1">
@@ -3584,8 +3609,8 @@
         <v>408</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="13" t="s">
+    <row r="26" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>410</v>
       </c>
       <c r="C26" s="1">
@@ -3601,8 +3626,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="13" t="s">
+    <row r="27" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>415</v>
       </c>
       <c r="C27" s="1">
@@ -3618,8 +3643,8 @@
         <v>418</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="13" t="s">
+    <row r="28" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>417</v>
       </c>
       <c r="C28" s="1">
@@ -3635,8 +3660,8 @@
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="13" t="s">
+    <row r="29" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>421</v>
       </c>
       <c r="C29" s="1">
@@ -3652,8 +3677,8 @@
         <v>425</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="13" t="s">
+    <row r="30" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>430</v>
       </c>
       <c r="C30" s="1">
@@ -3669,8 +3694,8 @@
         <v>429</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="13" t="s">
+    <row r="31" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>422</v>
       </c>
       <c r="C31" s="1">
@@ -3686,8 +3711,8 @@
         <v>433</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="13" t="s">
+    <row r="32" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>423</v>
       </c>
       <c r="C32" s="1">
@@ -3703,19 +3728,35 @@
         <v>434</v>
       </c>
     </row>
-    <row r="33" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C33" s="3">
+        <v>104</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:6" ht="57.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3730,15 +3771,15 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="7" width="28.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3755,7 +3796,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -3772,7 +3813,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -3789,7 +3830,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>144</v>
       </c>
@@ -3806,7 +3847,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>303</v>
       </c>
@@ -3823,7 +3864,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>343</v>
       </c>
@@ -3840,7 +3881,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>378</v>
       </c>
@@ -3857,23 +3898,23 @@
         <v>380</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:6" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="56.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 3 LCs and 8 SUs, also fixed scrolling too far east/west resulting in loss of markers (thanks Ro)
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAA3495-761B-4C4D-89B9-A5A3CA9D887C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBC620F-0892-4B8D-AFCA-458EEBB66882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="4180" yWindow="1160" windowWidth="19380" windowHeight="19720" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="489">
   <si>
     <t>Company Name</t>
   </si>
@@ -1379,6 +1379,139 @@
   </si>
   <si>
     <t>Allegro EU</t>
+  </si>
+  <si>
+    <t>Foxconn</t>
+  </si>
+  <si>
+    <t>high-speed optical transceiver modules (800G and 1.6T) utilizing POET’s Optical Interposer™ technology for AI Data Centers</t>
+  </si>
+  <si>
+    <t>CEO: Brand Cheng and Young Liu</t>
+  </si>
+  <si>
+    <t>Shenzhen, China and New Taipei City, Taiwan and New Delhi, India</t>
+  </si>
+  <si>
+    <t>CEO: Yaniv Ben-Haim, CTO: Prof. Yosef Ben-Ezra, VP of R&amp;D: Oren Horvits</t>
+  </si>
+  <si>
+    <t>All-Optical Chips for Digital Signal Processing,  Linear-drive Pluggable Optics (LPO), Co-packaged Optics (CPO), and All-Optics Switch Fabric</t>
+  </si>
+  <si>
+    <t>NewPhotonics</t>
+  </si>
+  <si>
+    <t>Douglas County, Colorado</t>
+  </si>
+  <si>
+    <t>Petah Tikva, Israel</t>
+  </si>
+  <si>
+    <t>Lightwave Logic, Inc.</t>
+  </si>
+  <si>
+    <t>next-generation Electro-Optic – “EO” – polymers modulators, high-effiecent 200 Gbps</t>
+  </si>
+  <si>
+    <t>CEO: Dr. Michael S. Lebby, Yves LeMaitre, VPE: Dr. John Zyskind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SilOriX </t>
+  </si>
+  <si>
+    <t>Karlsruhe Institute of Technology (KIT), CEO: Dr. Adrian Mertens, CTO: Dr. Carsten Eschenbaum</t>
+  </si>
+  <si>
+    <t>Karlsruhe, Germany</t>
+  </si>
+  <si>
+    <t>energy-efficient electro-optic modulators using Silicon Organic Hybrid (SOH) technology. Vpi &lt; 1V, BW 50GHz, 1250nm - 1650nm</t>
+  </si>
+  <si>
+    <t>Soitec</t>
+  </si>
+  <si>
+    <t>SOI and InP substrates</t>
+  </si>
+  <si>
+    <t>CEO: Pierre Barnabé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bernin, France and Gloucester, Massachusetts, USA and Singapore and Shanghai, China and Tokyo, Japan and Hwaseong-si, South Korea and Zhubei, Taiwan  </t>
+  </si>
+  <si>
+    <t>VIGO Photonics</t>
+  </si>
+  <si>
+    <t>photonic integrated circuits (PICs) for mid-infrared sensing applications (HyperPIC Project) . integrating signal processing into its sensor platforms</t>
+  </si>
+  <si>
+    <t>CEO: Dr. Adam Piotrowski, COO: Marcin Szrom</t>
+  </si>
+  <si>
+    <t>Founders: Zaijun Chen, Ryan Hamerly, Mengjie Yu, Dirk Englund Affliations: UC Berkeley, MIT, NTT</t>
+  </si>
+  <si>
+    <t>AI Computing With Photonic Chip. We accelerate AI computing with 100x energy efficiency and chip computing density. 5M USD Seed Funding</t>
+  </si>
+  <si>
+    <t>Opticore</t>
+  </si>
+  <si>
+    <t>Fremont, California, USA</t>
+  </si>
+  <si>
+    <t>CogniFiber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiber-Based Optical AI Computing, 1000x faster, 100x more efficient, </t>
+  </si>
+  <si>
+    <t>Rosh HaAyin, Israel</t>
+  </si>
+  <si>
+    <t>Founders: Dr. Eyal Cohen, Prof. Zeev Zalevsky, Affliations: Bar-Ilan University</t>
+  </si>
+  <si>
+    <t>Brightlight Photonics</t>
+  </si>
+  <si>
+    <t>Ti:Sapphire On-Chip Lasers and Amplifiers: Creating high-gain titanium-doped thin-film sapphire devices that are widely tunable (&gt;200 nm), single-frequency laser arrays (power &gt;10 mW, linewidth &lt;5 kHz), and amplifiers (power &gt;100 mW).  Ultra-Low-Loss UV and Visible Photonics: Offering custom photonic solutions with waveguide propagation losses as low as &lt;1 dB/m at 780 nm and &lt;10 dB/m at 400 nm</t>
+  </si>
+  <si>
+    <t>CEO: Joshua Yang and Alex Place</t>
+  </si>
+  <si>
+    <t>Cambridge,
+Massachusetts, USA</t>
+  </si>
+  <si>
+    <t>Marvell Technology</t>
+  </si>
+  <si>
+    <t>3D Silicon Photonics Engine, 1.6T Silicon Photonics Light Engine, 1.6T Silicon Photonics Light Engine</t>
+  </si>
+  <si>
+    <t>CEO: Matt Murphy, CTO Optical Engineering: Dr. Radha Nagarajan</t>
+  </si>
+  <si>
+    <t>Santa Clara, California, USA and Ottawa, Canada</t>
+  </si>
+  <si>
+    <t>AttoTude</t>
+  </si>
+  <si>
+    <t>silicon photonics to address the challenges of high-speed networking in AI and hyperscale data centers, 40M USD</t>
+  </si>
+  <si>
+    <t>Founders:  Dr. Dave Welch and Dr. Joy Laskar</t>
+  </si>
+  <si>
+    <t>Menlo Park, California, USA</t>
+  </si>
+  <si>
+    <t>Tomaszow Mazowiecki, Poland and St. Petersburg, Florida, USA and Taipei, Taiwan</t>
   </si>
 </sst>
 </file>
@@ -1398,6 +1531,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1824,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
@@ -2671,14 +2805,142 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="52" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="53" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="54" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="55" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="56" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="57" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="58" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="51" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="C51" s="3">
+        <v>26</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C52" s="3">
+        <v>21</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C53" s="3">
+        <v>5</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="C54" s="3">
+        <v>207</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C55" s="3">
+        <v>10</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B56" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="C56" s="3">
+        <v>13</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="C57" s="3">
+        <v>5</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="C58" s="3">
+        <v>50</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
     <row r="59" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="60" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="61" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2731,8 +2993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A24" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -3185,21 +3447,69 @@
         <v>387</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="29" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="30" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2300</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C30" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
     <row r="31" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="32" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="33" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="33" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="37" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="38" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="39" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="40" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="43" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="44" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="45" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
added 5 SU and 2 LC
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBC620F-0892-4B8D-AFCA-458EEBB66882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D21458-9254-4E11-A967-4EA2F82F0C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="1160" windowWidth="19380" windowHeight="19720" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="514">
   <si>
     <t>Company Name</t>
   </si>
@@ -450,9 +450,6 @@
   </si>
   <si>
     <t>Advanced heterogeneous integration, SiN, GaAs, GaN, InP</t>
-  </si>
-  <si>
-    <t>&lt;200</t>
   </si>
   <si>
     <t>Aachen, Germany</t>
@@ -1512,6 +1509,84 @@
   </si>
   <si>
     <t>Tomaszow Mazowiecki, Poland and St. Petersburg, Florida, USA and Taipei, Taiwan</t>
+  </si>
+  <si>
+    <t>AuthenX Inc</t>
+  </si>
+  <si>
+    <t>Si Ph and IIIV Ph for Co-Packaged Optics (CPO) Switches, Si Ph Interconnects for AI GPU. Fiber to the x</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Hsinchu, Taiwan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Silicon Photonics for Fiber Sensing</t>
+  </si>
+  <si>
+    <t>CEO: Leendert-Jan Nijstad and CTO:  Nick Singh</t>
+  </si>
+  <si>
+    <t>Alkmaar, Netherlands and Eindhoven, Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PhotonFirst </t>
+  </si>
+  <si>
+    <t>LuxQuanta</t>
+  </si>
+  <si>
+    <t>Continuous Variable Quantum Key Distribution (CV-QKD) systems. integrated photonics-based CV-QKD systems. Their flagship product, NOVA LQ®, is designed for secure, long-distance communication</t>
+  </si>
+  <si>
+    <t>CEO: Vanesa Díaz and CTO: Dr. Sebastián Etcheverry, Affliations: Institute of Photonic Sciences (ICFO)</t>
+  </si>
+  <si>
+    <t>Castelldefels, Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sicoya GmbH </t>
+  </si>
+  <si>
+    <t>monolithically integrated SiPh optical transceivers for data center and telecom</t>
+  </si>
+  <si>
+    <t>CEO Dr. Sven Otte. CTO: Dr. Stefan Meister, Dr. Hanjo Rhee</t>
+  </si>
+  <si>
+    <t>world's smallest laser integrated on silicon—500 times smaller than industry standards. enables ultra-dense integration (&gt;10,000 devices/mm²) and unmatched energy efficiency (&lt;0.1 pJ/bit),</t>
+  </si>
+  <si>
+    <t>CEO: Dr. Francesco Manegatti, CTO: Dr. Bruno Garbin</t>
+  </si>
+  <si>
+    <t>NcodiN</t>
+  </si>
+  <si>
+    <t>InnoLight Technology</t>
+  </si>
+  <si>
+    <t>Si Ph 800G High-Speed Optical Transceivers</t>
+  </si>
+  <si>
+    <t>CEO: Dr. Sheng Liu, VP R&amp;D: Dr. Charlie X. Wang, CTO: Oliver Sun</t>
+  </si>
+  <si>
+    <t>Jiangsu Province, China and Santa Carla, California, USA and Beijing, China and Shenzhen, China and Chengdu, China</t>
+  </si>
+  <si>
+    <t>Eoptolink Technology Inc., Ltd.</t>
+  </si>
+  <si>
+    <t>Si Ph high-speed optical transcievers</t>
+  </si>
+  <si>
+    <t>CEO: Richard Huang, President: Xiaolei Huang</t>
+  </si>
+  <si>
+    <t>Chengdu, China and Fremont, California, USA and Singapore</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1620,6 +1695,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1958,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
@@ -1986,7 +2064,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2003,7 +2081,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2020,7 +2098,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2173,7 +2251,7 @@
         <v>58</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2187,7 +2265,7 @@
         <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>60</v>
@@ -2218,13 +2296,13 @@
         <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>63</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2275,7 +2353,7 @@
         <v>85</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2360,7 +2438,7 @@
         <v>109</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2377,7 +2455,7 @@
         <v>112</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2411,7 +2489,7 @@
         <v>117</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2462,7 +2540,7 @@
         <v>133</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2476,330 +2554,330 @@
         <v>136</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C33" s="3">
         <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C34" s="3">
         <v>190</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B35" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C35" s="3">
         <v>30</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C36" s="3">
         <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C37" s="3">
         <v>40</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C38" s="3">
         <v>30</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B39" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C39" s="11">
         <v>50</v>
       </c>
       <c r="D39" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>335</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B40" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C40" s="3">
         <v>20</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>350</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C41" s="3">
         <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B42" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C42" s="3">
         <v>120</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B43" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C43" s="3">
         <v>20</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B44" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C44" s="3">
         <v>50</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C45" s="3">
         <v>20</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C46" s="3">
         <v>50</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C47" s="3">
         <v>150</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C48" s="3">
         <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>394</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C49" s="3">
         <v>104</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>440</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C50" s="3">
         <v>50</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>442</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>443</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>60</v>
@@ -2807,145 +2885,225 @@
     </row>
     <row r="51" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C51" s="3">
         <v>26</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C52" s="3">
         <v>21</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>456</v>
-      </c>
       <c r="F52" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C53" s="3">
         <v>5</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B54" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C54" s="3">
         <v>207</v>
       </c>
       <c r="D54" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>467</v>
-      </c>
       <c r="F54" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B55" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C55" s="3">
         <v>10</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B56" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C56" s="3">
         <v>13</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C57" s="3">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B58" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C58" s="3">
         <v>50</v>
       </c>
       <c r="D58" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="60" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="61" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="62" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="63" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    </row>
+    <row r="59" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B59" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B60" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B61" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="C61" s="3">
+        <v>50</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B63" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
     <row r="64" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="65" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="66" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2993,526 +3151,559 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="28.08203125" style="3" customWidth="1"/>
+    <col min="4" max="7" width="28.08203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="3">
+        <v>500</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3">
+        <v>700</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3">
+        <v>470</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1500</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="13">
+        <v>30000</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="13">
+        <v>5000</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="13">
+        <v>8000</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="D12" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="13">
+        <v>700</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C14" s="3">
+        <v>800</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1400</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C16" s="3">
         <v>500</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="3">
+        <v>100</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="3">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="13">
+        <v>15000</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1">
-        <v>700</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="1">
-        <v>470</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1500</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="5">
-        <v>30000</v>
-      </c>
-      <c r="D9" s="1" t="s">
+    <row r="20" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="3">
+        <v>14000</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="C21" s="3">
+        <v>300</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C22" s="3">
+        <v>500</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C23" s="3">
+        <v>100</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C24" s="3">
+        <v>500</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C25" s="3">
+        <v>200</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C26" s="3">
+        <v>400</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C27" s="3">
+        <v>500</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2300</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="C30" s="3">
         <v>5000</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="5">
-        <v>8000</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="1">
-        <v>150</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="5">
-        <v>700</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C14" s="1">
-        <v>800</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1400</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C16" s="1">
-        <v>500</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="1">
-        <v>100</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="1">
-        <v>30</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="5">
-        <v>15000</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="1">
-        <v>14000</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C21" s="1">
-        <v>300</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C22" s="1">
-        <v>500</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C23" s="1">
-        <v>100</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C24" s="1">
-        <v>500</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C25" s="1">
-        <v>200</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C26" s="1">
-        <v>400</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="C27" s="1">
-        <v>500</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2000</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="C29" s="1">
-        <v>2300</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="C30" s="1">
-        <v>5000</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="32" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="33" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" s="1" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" ht="59.15" customHeight="1" x14ac:dyDescent="0.4"/>
+    </row>
+    <row r="31" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B31" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="C31" s="13">
+        <v>1294</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="C32" s="13">
+        <v>1933</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="33" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="34" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="35" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="36" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="37" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="38" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="39" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="40" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="41" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="42" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="43" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="44" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="45" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3522,8 +3713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3E1C2-3C44-2549-B6BE-21FD6EE1DD33}">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -3550,7 +3741,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
@@ -3561,47 +3752,47 @@
         <v>13000</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>181</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" s="1">
         <v>500</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1">
         <v>130</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
@@ -3609,16 +3800,16 @@
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
@@ -3626,50 +3817,50 @@
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C8" s="1">
         <v>70</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>199</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C9" s="5">
         <v>10000</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="F9" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
@@ -3680,7 +3871,7 @@
         <v>100</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>96</v>
@@ -3694,16 +3885,16 @@
         <v>77</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
@@ -3714,214 +3905,214 @@
         <v>5500</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>214</v>
-      </c>
       <c r="F12" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="F13" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" s="5">
         <v>4500</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>220</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" s="1">
         <v>20</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C16" s="1">
         <v>20</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C17" s="1">
         <v>150</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>250</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C18" s="1">
         <v>1000</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C19" s="1">
         <v>20</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>333</v>
-      </c>
       <c r="F19" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C20" s="1">
         <v>50</v>
       </c>
       <c r="D20" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>335</v>
-      </c>
       <c r="F20" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C21" s="1">
         <v>50</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="E22" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>401</v>
-      </c>
       <c r="F22" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C23" s="1">
         <v>100</v>
       </c>
       <c r="D23" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>404</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C24" s="1">
         <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>121</v>
@@ -3929,155 +4120,155 @@
     </row>
     <row r="25" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C25" s="1">
         <v>20</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>407</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C26" s="1">
         <v>1000</v>
       </c>
       <c r="D26" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>411</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C27" s="1">
         <v>200</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C28" s="1">
         <v>10</v>
       </c>
       <c r="D28" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>420</v>
-      </c>
       <c r="F28" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C29" s="1">
         <v>35</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>424</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C30" s="1">
         <v>80</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>428</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C31" s="1">
         <v>20</v>
       </c>
       <c r="D31" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>432</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C32" s="1">
         <v>40</v>
       </c>
       <c r="D32" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>436</v>
-      </c>
       <c r="F32" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C33" s="3">
         <v>104</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -4102,154 +4293,156 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D8C265-B588-454D-B906-8DDBB021B0D6}">
   <dimension ref="B1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="28.08203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40" style="1" customWidth="1"/>
+    <col min="5" max="7" width="28.08203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>145</v>
+      <c r="C3" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C6" s="3">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C6" s="1">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="3">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C7" s="1">
-        <v>50</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C8" s="3">
+        <v>300</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C8" s="1">
-        <v>300</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.4"/>
+    </row>
+    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 7 start ups, and updated 2, e.g. Scantinel's Unsolvency as report by photonics.com
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D21458-9254-4E11-A967-4EA2F82F0C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE710EE-F574-4269-B8DD-BCB2ECC54F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="20840" yWindow="3660" windowWidth="16020" windowHeight="13480" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="543">
   <si>
     <t>Company Name</t>
   </si>
@@ -940,12 +940,6 @@
     <t>Arago</t>
   </si>
   <si>
-    <t>Si Photonics for AI acceleration (in stealth)</t>
-  </si>
-  <si>
-    <t>Hans-Christian Boos</t>
-  </si>
-  <si>
     <t>Paris, France and San Francisco, California</t>
   </si>
   <si>
@@ -1587,13 +1581,119 @@
   </si>
   <si>
     <t>Chengdu, China and Fremont, California, USA and Singapore</t>
+  </si>
+  <si>
+    <t>James Lee (CEO), Matthew Anderson (CSO), and Mateusz Kubica (CTO), University of Cambridge’s Toshiba Quantum Information Group</t>
+  </si>
+  <si>
+    <t>Cambridge, United Kingdom</t>
+  </si>
+  <si>
+    <t>Wave Photonics</t>
+  </si>
+  <si>
+    <t>computational design tools and services to dramatically speed up the photonic integrated circuit (PIC) development cycle, Packaging</t>
+  </si>
+  <si>
+    <t>Saint‑Sulpice, Switzerland</t>
+  </si>
+  <si>
+    <t>Luxtelligence</t>
+  </si>
+  <si>
+    <t>thin‑film lithium niobate (TFLN) and lithium tantalate (TFLT) photonics.</t>
+  </si>
+  <si>
+    <t>&lt; 10</t>
+  </si>
+  <si>
+    <t>Mohammad Bereyhi, CEO &amp; Co‑Founder. Alberto Beccari, CTO, EPFL spinout</t>
+  </si>
+  <si>
+    <t>Luceda Photonics</t>
+  </si>
+  <si>
+    <t>Pieter Dumon, Joris Geessels, and Martin Fiers, Photonics Research Group at Ghent University (UGent), the B‑PHOT lab at the Vrije Universiteit Brussel (VUB), and IMEC</t>
+  </si>
+  <si>
+    <t>Dendermonde, Belgium</t>
+  </si>
+  <si>
+    <t>photonic integrated circuit (PIC) design software and simulation services</t>
+  </si>
+  <si>
+    <t>Scantinel Photonics</t>
+  </si>
+  <si>
+    <t>Andy Zott — CTO &amp; Co‑Founder, Vladimir Davydenko — Co‑Founder</t>
+  </si>
+  <si>
+    <t>Ulm, Germany</t>
+  </si>
+  <si>
+    <t>Milan, Italy</t>
+  </si>
+  <si>
+    <t>Andrea Rocchetto — CEO and Co-founder</t>
+  </si>
+  <si>
+    <t>Glass-based photonic chips for quantum computing, communications, sensing, energy-efficient classical compute</t>
+  </si>
+  <si>
+    <t>Ephos</t>
+  </si>
+  <si>
+    <t>CEO: Nicolas Muller; Co-CTOs: Eliott Sarrey &amp; Ambroise Müller</t>
+  </si>
+  <si>
+    <t>Si Photonics for AI acceleration , Photonic–electronic AI inference chip ("JEF") for 10× lower energy use</t>
+  </si>
+  <si>
+    <t>CEO &amp; Founder: Tapa Ghosh, CTO &amp; Co‑Founder: Roy Meade, backers include Sam Altman, Alex Wang (Scale AI founder), Trevor Blackwell (Y Combinator)</t>
+  </si>
+  <si>
+    <t>San Mateo, California, USA</t>
+  </si>
+  <si>
+    <t>Photonic compute platform: direct laser modulation + on-chip waveguides, Photonic Motherboard for AI: high bandwidth, low power, efficient interconnects</t>
+  </si>
+  <si>
+    <t>Volantis</t>
+  </si>
+  <si>
+    <t>Avicena</t>
+  </si>
+  <si>
+    <t>Founder &amp; CEO: Dr. Bardia Pezeshki. CTO &amp; Co-Founder: Rob Kalman</t>
+  </si>
+  <si>
+    <t>Sunnyvale, California and Edinburgh, Scotland</t>
+  </si>
+  <si>
+    <t>MicroLED-based optical interconnects (LightBundle™) for AI/HPC/memory systems</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Frequency-Modulated Continuous-Wave (FMCW) LiDAR, leveraging photonic integrated circuits (PICs) to deliver long-range (300 m+), highly integrated, solid-state LiDAR solutions, single-chip scanner-detector PIC </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FILED FOR INSOLVENCY: 8/25</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1638,6 +1738,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1659,7 +1767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1699,6 +1807,9 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2036,8 +2147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
@@ -2636,248 +2747,248 @@
         <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C37" s="3">
         <v>40</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C38" s="3">
         <v>30</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B39" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C39" s="11">
         <v>50</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B40" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C40" s="3">
         <v>20</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C41" s="3">
         <v>81</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="F41" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B42" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C42" s="3">
         <v>120</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B43" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C43" s="3">
         <v>20</v>
       </c>
       <c r="D43" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B44" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C44" s="3">
         <v>50</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C45" s="3">
         <v>20</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C46" s="3">
         <v>50</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C47" s="3">
         <v>150</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C48" s="3">
         <v>3</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="3" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C49" s="3">
         <v>104</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="3" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C50" s="3">
         <v>50</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>60</v>
@@ -2885,203 +2996,203 @@
     </row>
     <row r="51" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C51" s="3">
         <v>26</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C52" s="3">
         <v>21</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="3" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C53" s="3">
         <v>5</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B54" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C54" s="3">
         <v>207</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B55" s="3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C55" s="3">
         <v>10</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B56" s="3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C56" s="3">
         <v>13</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>474</v>
-      </c>
       <c r="F56" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="3" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C57" s="3">
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B58" s="3" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C58" s="3">
         <v>50</v>
       </c>
       <c r="D58" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>484</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="59" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B59" s="3" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D59" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="60" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B60" s="3" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="61" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B61" s="3" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C61" s="3">
         <v>50</v>
       </c>
       <c r="D61" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="62" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B62" s="3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>60</v>
@@ -3089,38 +3200,150 @@
     </row>
     <row r="63" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B63" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="65" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="66" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="67" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="68" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="69" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="70" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="71" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="72" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="73" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="74" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="77" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="78" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="79" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="64" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B64" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="C64" s="3">
+        <v>30</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B65" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B66" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B67" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B68" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="C68" s="3">
+        <v>18</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B69" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B70" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="73" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="74" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="77" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="78" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="79" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="80" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="81" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="82" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="83" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3151,8 +3374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCED6EBF-A516-2344-ACEF-C5C6F963DECA}">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
@@ -3515,7 +3738,7 @@
         <v>242</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>251</v>
@@ -3523,33 +3746,33 @@
     </row>
     <row r="23" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C23" s="3">
         <v>100</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C24" s="3">
         <v>500</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>177</v>
@@ -3557,138 +3780,138 @@
     </row>
     <row r="25" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C25" s="3">
         <v>200</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C26" s="3">
         <v>400</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>341</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C27" s="3">
         <v>500</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C28" s="3">
         <v>2000</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C29" s="3">
         <v>2300</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B30" s="3" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C30" s="3">
         <v>5000</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B31" s="3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C31" s="13">
         <v>1294</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="3" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C32" s="13">
         <v>1933</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>511</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="33" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3713,8 +3936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3E1C2-3C44-2549-B6BE-21FD6EE1DD33}">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -4001,33 +4224,33 @@
     </row>
     <row r="18" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C18" s="1">
         <v>1000</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E18" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>311</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C19" s="1">
         <v>20</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>200</v>
@@ -4035,50 +4258,50 @@
     </row>
     <row r="20" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C20" s="1">
         <v>50</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E20" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>334</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C21" s="1">
         <v>50</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>398</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>400</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>152</v>
@@ -4086,33 +4309,33 @@
     </row>
     <row r="23" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C23" s="1">
         <v>100</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C24" s="1">
         <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>121</v>
@@ -4120,67 +4343,67 @@
     </row>
     <row r="25" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C25" s="1">
         <v>20</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>408</v>
-      </c>
       <c r="F25" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C26" s="1">
         <v>1000</v>
       </c>
       <c r="D26" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>412</v>
-      </c>
       <c r="F26" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C27" s="1">
         <v>200</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>415</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C28" s="1">
         <v>10</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>200</v>
@@ -4188,87 +4411,87 @@
     </row>
     <row r="29" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C29" s="1">
         <v>35</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>425</v>
-      </c>
       <c r="F29" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C30" s="1">
         <v>80</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>426</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>427</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C31" s="1">
         <v>20</v>
       </c>
       <c r="D31" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>430</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C32" s="1">
         <v>40</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="3" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C33" s="3">
         <v>104</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -4377,53 +4600,53 @@
     </row>
     <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C6" s="3">
         <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C7" s="3">
         <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C8" s="3">
         <v>300</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added 5 SUs, and 1 Foundry
</commit_message>
<xml_diff>
--- a/Photonic Companies.xlsx
+++ b/Photonic Companies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blow\CodingProjects\PhotonicCompanies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blow/Desktop/GitHub/PhotonicCompanies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE710EE-F574-4269-B8DD-BCB2ECC54F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8A6D29-EAA1-4F41-B691-D41504F45002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20840" yWindow="3660" windowWidth="16020" windowHeight="13480" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EBDBD758-277E-6B49-B4C7-31ED6652B0E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="566">
   <si>
     <t>Company Name</t>
   </si>
@@ -1687,6 +1687,75 @@
       </rPr>
       <t>FILED FOR INSOLVENCY: 8/25</t>
     </r>
+  </si>
+  <si>
+    <t>Sabratha Photonics</t>
+  </si>
+  <si>
+    <t>thin-film lithium niobate (TFLN) photonic platform, building blocks include tunable microring resonators (high-Q), ultra-high-speed electro-optic modulators (targeting 5G/6G telecom and datacenter applications), plus Brillouin-active spirals for narrow-band amplification / optical-RF filter functions</t>
+  </si>
+  <si>
+    <t>Spin-out from University of Twente (UT), Kees Franken (CEO), Steven Ye (CTO), David Marpaung (Chief Scientist)</t>
+  </si>
+  <si>
+    <t>MetaLenX</t>
+  </si>
+  <si>
+    <t>The company focuses on metalens / metasurface optics: design, manufacturing, and industrialization of metalens devices, 13.7 M USD Raised</t>
+  </si>
+  <si>
+    <t>Shenzhen, China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown </t>
+  </si>
+  <si>
+    <t>New Silicon Corporation (nsc)</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the first to “monolithically integrate compound semiconductors with silicon CMOS” at full wafer scale, rather than relying on packaging or hybrid stacking. embed III-V devices with CMOS Silicon </t>
+  </si>
+  <si>
+    <t>Chairman: Eugene (Gene) Fitzgerald; CEO: Dr. Andrew Kim; Chief Scientist: Dr. Kenneth Lee</t>
+  </si>
+  <si>
+    <t>Austin, Texas, USA</t>
+  </si>
+  <si>
+    <t>Neurophos</t>
+  </si>
+  <si>
+    <t>optical processing units (OPUs) based on metasurface + silicon photonics — using optical modulators built from metamaterials and photonics rather than traditional electronic transistors; claim modulators 10,000x time smaller than SoTA, with 300 TOPS/W</t>
+  </si>
+  <si>
+    <t>Patrick Bown (CEO), Hod Finkelstein (CTO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Broomfield, Colorado, USA</t>
+  </si>
+  <si>
+    <t>Polaris Electro-Optics, Inc.</t>
+  </si>
+  <si>
+    <t>Affliation: University of Colorado Boulder, Morten Nissov (CEO), Cory Pecinovsky (CTO)</t>
+  </si>
+  <si>
+    <t>Polaris is developing a novel electro-optic modulator platform based on proprietary ferroelectric nematic glass / liquid-crystal materials, Datacenters, High Performance Computing</t>
+  </si>
+  <si>
+    <t>Chongqing, China</t>
+  </si>
+  <si>
+    <t>China United Microelectronics Center (CUMEC)</t>
+  </si>
+  <si>
+    <t>government-backed microelectronics and silicon-photonics R&amp;D + pilot-manufacturing center.silicon photonics, heterogeneous 3D integration, SiGe RF, and other “More-than-Moore” technologies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jin Guo (Managing Director) </t>
   </si>
 </sst>
 </file>
@@ -1767,7 +1836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1807,9 +1876,6 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2147,21 +2213,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9869D2E4-4022-4440-93A4-7A77C39B4047}">
   <dimension ref="B1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F76" sqref="B76:F76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="28.08203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="45.25" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.08203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="28" style="3" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="28" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2178,7 +2244,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -2195,7 +2261,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -2212,7 +2278,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -2229,7 +2295,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2246,7 +2312,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
@@ -2263,7 +2329,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -2280,7 +2346,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -2297,7 +2363,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
@@ -2314,7 +2380,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
@@ -2331,7 +2397,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -2348,7 +2414,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
@@ -2365,7 +2431,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -2382,7 +2448,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -2399,7 +2465,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>62</v>
       </c>
@@ -2416,7 +2482,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
@@ -2433,7 +2499,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
@@ -2450,7 +2516,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>83</v>
       </c>
@@ -2467,7 +2533,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
@@ -2484,7 +2550,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
@@ -2501,7 +2567,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>97</v>
       </c>
@@ -2518,7 +2584,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
@@ -2535,7 +2601,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>106</v>
       </c>
@@ -2552,7 +2618,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
@@ -2569,7 +2635,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>113</v>
       </c>
@@ -2586,7 +2652,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>116</v>
       </c>
@@ -2603,7 +2669,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>120</v>
       </c>
@@ -2620,7 +2686,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>124</v>
       </c>
@@ -2637,7 +2703,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>131</v>
       </c>
@@ -2654,7 +2720,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
@@ -2671,7 +2737,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>148</v>
       </c>
@@ -2688,7 +2754,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>243</v>
       </c>
@@ -2705,7 +2771,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>290</v>
       </c>
@@ -2722,7 +2788,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>293</v>
       </c>
@@ -2739,7 +2805,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>298</v>
       </c>
@@ -2756,7 +2822,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>304</v>
       </c>
@@ -2773,7 +2839,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>312</v>
       </c>
@@ -2790,7 +2856,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
         <v>333</v>
       </c>
@@ -2807,7 +2873,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>344</v>
       </c>
@@ -2824,7 +2890,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
         <v>348</v>
       </c>
@@ -2841,7 +2907,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>352</v>
       </c>
@@ -2858,7 +2924,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>356</v>
       </c>
@@ -2875,7 +2941,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>360</v>
       </c>
@@ -2892,7 +2958,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>367</v>
       </c>
@@ -2909,7 +2975,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>371</v>
       </c>
@@ -2926,7 +2992,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>382</v>
       </c>
@@ -2943,7 +3009,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>387</v>
       </c>
@@ -2960,7 +3026,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>435</v>
       </c>
@@ -2977,7 +3043,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>441</v>
       </c>
@@ -2994,7 +3060,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>448</v>
       </c>
@@ -3011,7 +3077,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>451</v>
       </c>
@@ -3028,7 +3094,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="53" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>454</v>
       </c>
@@ -3045,7 +3111,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>462</v>
       </c>
@@ -3062,7 +3128,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>467</v>
       </c>
@@ -3079,7 +3145,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>469</v>
       </c>
@@ -3096,7 +3162,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>473</v>
       </c>
@@ -3113,7 +3179,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
         <v>481</v>
       </c>
@@ -3130,7 +3196,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>486</v>
       </c>
@@ -3147,7 +3213,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>493</v>
       </c>
@@ -3164,7 +3230,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>494</v>
       </c>
@@ -3181,7 +3247,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>498</v>
       </c>
@@ -3198,7 +3264,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>503</v>
       </c>
@@ -3215,7 +3281,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>514</v>
       </c>
@@ -3232,7 +3298,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>517</v>
       </c>
@@ -3245,11 +3311,11 @@
       <c r="E65" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="F65" s="14" t="s">
+      <c r="F65" s="1" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>521</v>
       </c>
@@ -3266,7 +3332,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>525</v>
       </c>
@@ -3283,7 +3349,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>531</v>
       </c>
@@ -3300,7 +3366,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
         <v>537</v>
       </c>
@@ -3317,7 +3383,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
         <v>538</v>
       </c>
@@ -3334,36 +3400,119 @@
         <v>540</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="72" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="73" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="74" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="77" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="78" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="79" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="82" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="85" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="86" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="89" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="91" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="92" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="93" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="94" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="95" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="96" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="97" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="99" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="100" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="71" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="C71" s="3">
+        <v>10</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="C72" s="3">
+        <v>20</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="C73" s="3">
+        <v>50</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="C74" s="3">
+        <v>22</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="C75" s="3">
+        <v>10</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3375,19 +3524,19 @@
   <dimension ref="B1:F45"/>
   <sheetViews>
     <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="28.08203125" style="3" customWidth="1"/>
-    <col min="4" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="28" style="3" customWidth="1"/>
+    <col min="4" max="7" width="28" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="59.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3404,7 +3553,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>161</v>
       </c>
@@ -3421,7 +3570,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
@@ -3438,7 +3587,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>255</v>
       </c>
@@ -3455,7 +3604,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
@@ -3472,7 +3621,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
@@ -3489,7 +3638,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
@@ -3506,7 +3655,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
@@ -3523,7 +3672,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3540,7 +3689,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>70</v>
       </c>
@@ -3557,7 +3706,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>71</v>
       </c>
@@ -3574,7 +3723,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>72</v>
       </c>
@@ -3591,7 +3740,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>279</v>
       </c>
@@ -3608,7 +3757,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>284</v>
       </c>
@@ -3625,7 +3774,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>268</v>
       </c>
@@ -3642,7 +3791,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>101</v>
       </c>
@@ -3659,7 +3808,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>102</v>
       </c>
@@ -3676,7 +3825,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>128</v>
       </c>
@@ -3693,7 +3842,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>130</v>
       </c>
@@ -3710,7 +3859,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>232</v>
       </c>
@@ -3727,7 +3876,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>241</v>
       </c>
@@ -3744,7 +3893,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>316</v>
       </c>
@@ -3761,7 +3910,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>322</v>
       </c>
@@ -3778,7 +3927,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>323</v>
       </c>
@@ -3795,7 +3944,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>338</v>
       </c>
@@ -3812,7 +3961,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>383</v>
       </c>
@@ -3829,7 +3978,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>442</v>
       </c>
@@ -3846,7 +3995,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>458</v>
       </c>
@@ -3863,7 +4012,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>477</v>
       </c>
@@ -3880,7 +4029,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>504</v>
       </c>
@@ -3897,7 +4046,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="59.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>508</v>
       </c>
@@ -3914,19 +4063,19 @@
         <v>511</v>
       </c>
     </row>
-    <row r="33" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="34" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="35" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="36" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="37" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="38" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="39" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="40" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="41" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="42" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="43" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="44" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="45" ht="59.15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="33" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3936,21 +4085,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C3E1C2-3C44-2549-B6BE-21FD6EE1DD33}">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="28.08203125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="28.08203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="28" style="1" customWidth="1"/>
+    <col min="4" max="6" width="28" style="7" customWidth="1"/>
+    <col min="7" max="7" width="28" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:6" s="12" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:6" s="12" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
@@ -3967,7 +4116,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -3984,7 +4133,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>182</v>
       </c>
@@ -4001,7 +4150,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>185</v>
       </c>
@@ -4018,7 +4167,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -4035,7 +4184,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
@@ -4052,7 +4201,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>199</v>
       </c>
@@ -4069,7 +4218,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>201</v>
       </c>
@@ -4086,7 +4235,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
@@ -4103,7 +4252,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>77</v>
       </c>
@@ -4120,7 +4269,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>123</v>
       </c>
@@ -4137,7 +4286,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>204</v>
       </c>
@@ -4154,7 +4303,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>207</v>
       </c>
@@ -4171,7 +4320,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>215</v>
       </c>
@@ -4188,7 +4337,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>239</v>
       </c>
@@ -4205,7 +4354,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>247</v>
       </c>
@@ -4222,7 +4371,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>308</v>
       </c>
@@ -4239,7 +4388,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>328</v>
       </c>
@@ -4256,7 +4405,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>333</v>
       </c>
@@ -4273,7 +4422,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>393</v>
       </c>
@@ -4290,7 +4439,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>396</v>
       </c>
@@ -4307,7 +4456,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>400</v>
       </c>
@@ -4324,7 +4473,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>364</v>
       </c>
@@ -4341,7 +4490,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>403</v>
       </c>
@@ -4358,7 +4507,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>407</v>
       </c>
@@ -4375,7 +4524,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>412</v>
       </c>
@@ -4392,7 +4541,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>414</v>
       </c>
@@ -4409,7 +4558,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>418</v>
       </c>
@@ -4426,7 +4575,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>427</v>
       </c>
@@ -4443,7 +4592,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>419</v>
       </c>
@@ -4460,7 +4609,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>420</v>
       </c>
@@ -4477,7 +4626,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>435</v>
       </c>
@@ -4494,18 +4643,34 @@
         <v>434</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C34" s="3">
+        <v>200</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="2:6" ht="58" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4520,17 +4685,17 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="19.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="28.08203125" style="3" customWidth="1"/>
+    <col min="2" max="3" width="28" style="3" customWidth="1"/>
     <col min="4" max="4" width="40" style="1" customWidth="1"/>
-    <col min="5" max="7" width="28.08203125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="28" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4547,7 +4712,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
@@ -4564,7 +4729,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -4581,7 +4746,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>143</v>
       </c>
@@ -4598,7 +4763,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>300</v>
       </c>
@@ -4615,7 +4780,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>340</v>
       </c>
@@ -4632,7 +4797,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>375</v>
       </c>
@@ -4649,23 +4814,23 @@
         <v>377</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="10" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="11" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="12" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="13" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="14" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="16" spans="2:6" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="17" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="18" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="19" ht="56.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="9" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="28" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="28" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="28" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="28" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="28" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="28" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>